<commit_message>
Simplify user testing template: clean sheet names and titles
- Sheet tabs now simply numbered: 1, 2, 3... 50
- Title on each sheet: "AEGIS Performance Testing" (no test numbers)
- Cleaner, more streamlined appearance

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/user_testing_template.xlsx
+++ b/user_testing_template.xlsx
@@ -7,56 +7,56 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 4" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 5" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 6" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 7" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 8" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 9" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 10" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 11" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 12" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 13" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 14" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 15" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 16" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 17" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 18" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 19" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 20" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 21" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 22" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 23" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 24" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 25" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 26" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 27" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 28" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 29" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 30" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 31" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 32" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 33" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 34" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 35" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 36" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 37" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 38" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 39" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 40" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 41" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 42" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 43" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 44" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 45" sheetId="45" state="visible" r:id="rId45"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 46" sheetId="46" state="visible" r:id="rId46"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 47" sheetId="47" state="visible" r:id="rId47"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 48" sheetId="48" state="visible" r:id="rId48"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 49" sheetId="49" state="visible" r:id="rId49"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test 50" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="6" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="7" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="8" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="9" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="10" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="12" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="13" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="14" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="15" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="16" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="17" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="18" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="19" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="21" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="22" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="23" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="24" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="25" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="26" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="27" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="28" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="29" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="30" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="31" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="32" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="33" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="34" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="35" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="36" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="37" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="38" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="39" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="40" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="41" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="42" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="43" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="44" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="45" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="46" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="47" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="48" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="49" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="50" sheetId="50" state="visible" r:id="rId50"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -551,7 +551,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #1</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #10</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -851,7 +851,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #11</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #12</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #13</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -1301,7 +1301,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #14</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -1451,7 +1451,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #15</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -1601,7 +1601,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #16</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -1751,7 +1751,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #17</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -1901,7 +1901,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #18</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -2051,7 +2051,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #19</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -2201,7 +2201,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #2</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -2351,7 +2351,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #20</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -2501,7 +2501,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #21</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -2651,7 +2651,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #22</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -2801,7 +2801,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #23</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -2951,7 +2951,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #24</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -3101,7 +3101,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #25</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -3251,7 +3251,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #26</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -3401,7 +3401,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #27</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -3551,7 +3551,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #28</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -3701,7 +3701,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #29</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -3851,7 +3851,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #3</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -4001,7 +4001,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #30</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -4151,7 +4151,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #31</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -4301,7 +4301,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #32</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -4451,7 +4451,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #33</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -4601,7 +4601,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #34</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -4751,7 +4751,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #35</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -4901,7 +4901,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #36</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -5051,7 +5051,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #37</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -5201,7 +5201,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #38</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -5351,7 +5351,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #39</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -5501,7 +5501,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #4</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -5651,7 +5651,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #40</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -5801,7 +5801,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #41</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -5951,7 +5951,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #42</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -6101,7 +6101,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #43</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -6251,7 +6251,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #44</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -6401,7 +6401,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #45</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -6551,7 +6551,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #46</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -6701,7 +6701,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #47</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -6851,7 +6851,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #48</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -7001,7 +7001,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #49</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -7151,7 +7151,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #5</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -7301,7 +7301,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #50</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -7451,7 +7451,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #6</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -7601,7 +7601,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #7</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -7751,7 +7751,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #8</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>
@@ -7901,7 +7901,7 @@
     <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AEGIS Performance Testing - Test #9</t>
+          <t>AEGIS Performance Testing</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add dropdown validation for easy database selection
Added Excel data validation dropdowns to database cells (D7:I7):
- Users click cell and select ✓ or X from dropdown
- Much easier than typing manually
- Cells styled with light gray background and 16pt font
- Clear visual indication of interactive cells

Note: True form control checkboxes require VBA macros which
openpyxl doesn't support, but dropdowns provide equivalent
easy-to-use functionality.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/user_testing_template.xlsx
+++ b/user_testing_template.xlsx
@@ -69,7 +69,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -114,8 +114,13 @@
       <name val="Calibri"/>
       <sz val="11"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="16"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -144,6 +149,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FFFFFF"/>
         <bgColor rgb="00FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F0F0F0"/>
+        <bgColor rgb="00F0F0F0"/>
       </patternFill>
     </fill>
   </fills>
@@ -266,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -323,6 +334,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -789,12 +803,12 @@
       <c r="A7" s="5" t="n"/>
       <c r="B7" s="5" t="n"/>
       <c r="C7" s="5" t="n"/>
-      <c r="D7" s="7" t="inlineStr"/>
-      <c r="E7" s="7" t="inlineStr"/>
-      <c r="F7" s="7" t="inlineStr"/>
-      <c r="G7" s="7" t="inlineStr"/>
-      <c r="H7" s="7" t="inlineStr"/>
-      <c r="I7" s="7" t="inlineStr"/>
+      <c r="D7" s="26" t="inlineStr"/>
+      <c r="E7" s="26" t="inlineStr"/>
+      <c r="F7" s="26" t="inlineStr"/>
+      <c r="G7" s="26" t="inlineStr"/>
+      <c r="H7" s="26" t="inlineStr"/>
+      <c r="I7" s="26" t="inlineStr"/>
     </row>
     <row r="8" ht="10" customHeight="1"/>
     <row r="9" ht="25" customHeight="1">
@@ -1790,6 +1804,11 @@
     <mergeCell ref="B10"/>
     <mergeCell ref="B9:C9"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation sqref="D7:I7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select ✓ or X" promptTitle="Database Selection" prompt="Click to select ✓ or X" type="list">
+      <formula1>"✓,X"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Fix alignment in database selection area
Removed borders from unused cells (A6-C7) to clean up layout.
Database selection now cleanly shows only the 6 database columns
(D-I) without wonky empty bordered cells on the left.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/user_testing_template.xlsx
+++ b/user_testing_template.xlsx
@@ -158,7 +158,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -273,11 +273,12 @@
       </bottom>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -337,6 +338,7 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -765,9 +767,9 @@
       <c r="I5" s="18" t="n"/>
     </row>
     <row r="6" ht="20" customHeight="1">
-      <c r="A6" s="5" t="n"/>
-      <c r="B6" s="5" t="n"/>
-      <c r="C6" s="5" t="n"/>
+      <c r="A6" s="27" t="n"/>
+      <c r="B6" s="27" t="n"/>
+      <c r="C6" s="27" t="n"/>
       <c r="D6" s="6" t="inlineStr">
         <is>
           <t>All</t>
@@ -800,9 +802,9 @@
       </c>
     </row>
     <row r="7" ht="25" customHeight="1">
-      <c r="A7" s="5" t="n"/>
-      <c r="B7" s="5" t="n"/>
-      <c r="C7" s="5" t="n"/>
+      <c r="A7" s="27" t="n"/>
+      <c r="B7" s="27" t="n"/>
+      <c r="C7" s="27" t="n"/>
       <c r="D7" s="26" t="inlineStr"/>
       <c r="E7" s="26" t="inlineStr"/>
       <c r="F7" s="26" t="inlineStr"/>

</xml_diff>

<commit_message>
Realign database selection to start at column A
Fixed alignment issue where database dropdowns were pushed to column D.
Now properly starts at column A:
- Row 5: Header merged A5:F5
- Row 6: Database labels in A-F (All, Supplementary, Pillar 3, Reports, RTS, Transcripts)
- Row 7: Dropdown checkboxes in A-F

Clean left-aligned layout matching the rest of the summary sheet.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/user_testing_template.xlsx
+++ b/user_testing_template.xlsx
@@ -278,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -339,6 +339,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -761,56 +764,53 @@
       <c r="C5" s="17" t="n"/>
       <c r="D5" s="17" t="n"/>
       <c r="E5" s="17" t="n"/>
-      <c r="F5" s="17" t="n"/>
-      <c r="G5" s="17" t="n"/>
-      <c r="H5" s="17" t="n"/>
-      <c r="I5" s="18" t="n"/>
+      <c r="F5" s="18" t="n"/>
     </row>
     <row r="6" ht="20" customHeight="1">
-      <c r="A6" s="27" t="n"/>
-      <c r="B6" s="27" t="n"/>
-      <c r="C6" s="27" t="n"/>
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>Supplementary</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="inlineStr">
+        <is>
+          <t>Pillar 3</t>
+        </is>
+      </c>
       <c r="D6" s="6" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Reports</t>
         </is>
       </c>
       <c r="E6" s="6" t="inlineStr">
         <is>
-          <t>Supplementary</t>
+          <t>RTS</t>
         </is>
       </c>
       <c r="F6" s="6" t="inlineStr">
         <is>
-          <t>Pillar 3</t>
-        </is>
-      </c>
-      <c r="G6" s="6" t="inlineStr">
-        <is>
-          <t>Reports</t>
-        </is>
-      </c>
-      <c r="H6" s="6" t="inlineStr">
-        <is>
-          <t>RTS</t>
-        </is>
-      </c>
-      <c r="I6" s="6" t="inlineStr">
-        <is>
           <t>Transcripts</t>
         </is>
       </c>
+      <c r="G6" s="28" t="n"/>
+      <c r="H6" s="28" t="n"/>
+      <c r="I6" s="28" t="n"/>
     </row>
     <row r="7" ht="25" customHeight="1">
-      <c r="A7" s="27" t="n"/>
-      <c r="B7" s="27" t="n"/>
-      <c r="C7" s="27" t="n"/>
+      <c r="A7" s="26" t="inlineStr"/>
+      <c r="B7" s="26" t="inlineStr"/>
+      <c r="C7" s="26" t="inlineStr"/>
       <c r="D7" s="26" t="inlineStr"/>
       <c r="E7" s="26" t="inlineStr"/>
       <c r="F7" s="26" t="inlineStr"/>
-      <c r="G7" s="26" t="inlineStr"/>
-      <c r="H7" s="26" t="inlineStr"/>
-      <c r="I7" s="26" t="inlineStr"/>
+      <c r="G7" s="28" t="n"/>
+      <c r="H7" s="28" t="n"/>
+      <c r="I7" s="28" t="n"/>
     </row>
     <row r="8" ht="10" customHeight="1"/>
     <row r="9" ht="25" customHeight="1">
@@ -1800,14 +1800,17 @@
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A5:F5"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B10"/>
     <mergeCell ref="B9:C9"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation sqref="D7:I7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select ✓ or X" promptTitle="Database Selection" prompt="Click to select ✓ or X" type="list">
+      <formula1>"✓,X"</formula1>
+    </dataValidation>
+    <dataValidation sqref="A7:F7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select ✓ or X" promptTitle="Database Selection" prompt="Click to select ✓ or X" type="list">
       <formula1>"✓,X"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Restructure summary with vertical database layout and aligned widths
Major layout improvements:
- Stack database dropdowns vertically (rows 6-11) instead of horizontally
- Align title, description, and database headers (all merge A:C)
- Fix sizing issues caused by wide question preview column
- Clean, professional vertical flow

Database selection now shows:
- Row 6-11: Database name (col A) + Dropdown (col B)
- Much better proportions and usability

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/user_testing_template.xlsx
+++ b/user_testing_template.xlsx
@@ -278,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -340,6 +340,25 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -707,7 +726,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -727,13 +746,29 @@
   </cols>
   <sheetData>
     <row r="1" ht="35" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="29" t="inlineStr">
         <is>
           <t>AEGIS Performance Testing - Summary</t>
         </is>
       </c>
-    </row>
-    <row r="2" ht="10" customHeight="1"/>
+      <c r="D1" s="30" t="n"/>
+      <c r="E1" s="30" t="n"/>
+      <c r="F1" s="30" t="n"/>
+      <c r="G1" s="30" t="n"/>
+      <c r="H1" s="30" t="n"/>
+      <c r="I1" s="30" t="n"/>
+    </row>
+    <row r="2" ht="10" customHeight="1">
+      <c r="A2" s="30" t="n"/>
+      <c r="B2" s="30" t="n"/>
+      <c r="C2" s="30" t="n"/>
+      <c r="D2" s="30" t="n"/>
+      <c r="E2" s="30" t="n"/>
+      <c r="F2" s="30" t="n"/>
+      <c r="G2" s="30" t="n"/>
+      <c r="H2" s="30" t="n"/>
+      <c r="I2" s="30" t="n"/>
+    </row>
     <row r="3" ht="30" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
@@ -745,309 +780,302 @@
           <t>Enter overall testing description here (e.g., Testing for Q3 earnings, Testing RTS functionality, etc.)</t>
         </is>
       </c>
-      <c r="C3" s="17" t="n"/>
-      <c r="D3" s="17" t="n"/>
-      <c r="E3" s="17" t="n"/>
-      <c r="F3" s="17" t="n"/>
-      <c r="G3" s="17" t="n"/>
-      <c r="H3" s="17" t="n"/>
-      <c r="I3" s="18" t="n"/>
-    </row>
-    <row r="4" ht="10" customHeight="1"/>
+      <c r="D3" s="30" t="n"/>
+      <c r="E3" s="30" t="n"/>
+      <c r="F3" s="30" t="n"/>
+      <c r="G3" s="30" t="n"/>
+      <c r="H3" s="30" t="n"/>
+      <c r="I3" s="30" t="n"/>
+    </row>
+    <row r="4" ht="10" customHeight="1">
+      <c r="A4" s="30" t="n"/>
+      <c r="B4" s="30" t="n"/>
+      <c r="C4" s="30" t="n"/>
+      <c r="D4" s="30" t="n"/>
+      <c r="E4" s="30" t="n"/>
+      <c r="F4" s="30" t="n"/>
+      <c r="G4" s="30" t="n"/>
+      <c r="H4" s="30" t="n"/>
+      <c r="I4" s="30" t="n"/>
+    </row>
     <row r="5" ht="25" customHeight="1">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>Database Selection (applies to all tests - check all that apply)</t>
-        </is>
-      </c>
-      <c r="B5" s="17" t="n"/>
-      <c r="C5" s="17" t="n"/>
-      <c r="D5" s="17" t="n"/>
-      <c r="E5" s="17" t="n"/>
-      <c r="F5" s="18" t="n"/>
-    </row>
-    <row r="6" ht="20" customHeight="1">
-      <c r="A6" s="6" t="inlineStr">
+          <t>Database Selection (applies to all tests)</t>
+        </is>
+      </c>
+      <c r="D5" s="30" t="n"/>
+      <c r="E5" s="30" t="n"/>
+      <c r="F5" s="30" t="n"/>
+      <c r="G5" s="30" t="n"/>
+      <c r="H5" s="30" t="n"/>
+      <c r="I5" s="30" t="n"/>
+    </row>
+    <row r="6" ht="25" customHeight="1">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>All</t>
         </is>
       </c>
-      <c r="B6" s="6" t="inlineStr">
-        <is>
-          <t>Supplementary</t>
-        </is>
-      </c>
-      <c r="C6" s="6" t="inlineStr">
-        <is>
-          <t>Pillar 3</t>
-        </is>
-      </c>
-      <c r="D6" s="6" t="inlineStr">
-        <is>
-          <t>Reports</t>
-        </is>
-      </c>
-      <c r="E6" s="6" t="inlineStr">
-        <is>
-          <t>RTS</t>
-        </is>
-      </c>
-      <c r="F6" s="6" t="inlineStr">
-        <is>
-          <t>Transcripts</t>
-        </is>
-      </c>
+      <c r="B6" s="31" t="inlineStr"/>
+      <c r="C6" s="28" t="n"/>
+      <c r="D6" s="28" t="n"/>
+      <c r="E6" s="28" t="n"/>
+      <c r="F6" s="28" t="n"/>
       <c r="G6" s="28" t="n"/>
       <c r="H6" s="28" t="n"/>
       <c r="I6" s="28" t="n"/>
     </row>
     <row r="7" ht="25" customHeight="1">
-      <c r="A7" s="26" t="inlineStr"/>
-      <c r="B7" s="26" t="inlineStr"/>
-      <c r="C7" s="26" t="inlineStr"/>
-      <c r="D7" s="26" t="inlineStr"/>
-      <c r="E7" s="26" t="inlineStr"/>
-      <c r="F7" s="26" t="inlineStr"/>
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>Supplementary</t>
+        </is>
+      </c>
+      <c r="B7" s="31" t="inlineStr"/>
+      <c r="C7" s="28" t="n"/>
+      <c r="D7" s="28" t="n"/>
+      <c r="E7" s="28" t="n"/>
+      <c r="F7" s="28" t="n"/>
       <c r="G7" s="28" t="n"/>
       <c r="H7" s="28" t="n"/>
       <c r="I7" s="28" t="n"/>
     </row>
-    <row r="8" ht="10" customHeight="1"/>
+    <row r="8" ht="25" customHeight="1">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Pillar 3</t>
+        </is>
+      </c>
+      <c r="B8" s="31" t="inlineStr"/>
+      <c r="C8" s="30" t="n"/>
+      <c r="D8" s="30" t="n"/>
+      <c r="E8" s="30" t="n"/>
+      <c r="F8" s="30" t="n"/>
+      <c r="G8" s="30" t="n"/>
+      <c r="H8" s="30" t="n"/>
+      <c r="I8" s="30" t="n"/>
+    </row>
     <row r="9" ht="25" customHeight="1">
-      <c r="A9" s="8" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>Reports</t>
+        </is>
+      </c>
+      <c r="B9" s="32" t="inlineStr"/>
+      <c r="C9" s="30" t="n"/>
+      <c r="D9" s="30" t="n"/>
+      <c r="E9" s="30" t="n"/>
+      <c r="F9" s="30" t="n"/>
+      <c r="G9" s="30" t="n"/>
+      <c r="H9" s="30" t="n"/>
+      <c r="I9" s="30" t="n"/>
+    </row>
+    <row r="10" ht="25" customHeight="1">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>RTS</t>
+        </is>
+      </c>
+      <c r="B10" s="31" t="inlineStr"/>
+      <c r="C10" s="28" t="n"/>
+      <c r="D10" s="30" t="n"/>
+      <c r="E10" s="30" t="n"/>
+      <c r="F10" s="30" t="n"/>
+      <c r="G10" s="30" t="n"/>
+      <c r="H10" s="30" t="n"/>
+      <c r="I10" s="30" t="n"/>
+    </row>
+    <row r="11" ht="25" customHeight="1">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>Transcripts</t>
+        </is>
+      </c>
+      <c r="B11" s="31" t="inlineStr"/>
+      <c r="C11" s="33" t="n"/>
+      <c r="D11" s="30" t="n"/>
+      <c r="E11" s="30" t="n"/>
+      <c r="F11" s="30" t="n"/>
+      <c r="G11" s="30" t="n"/>
+      <c r="H11" s="30" t="n"/>
+      <c r="I11" s="30" t="n"/>
+    </row>
+    <row r="12" ht="10" customHeight="1">
+      <c r="A12" s="28" t="n"/>
+      <c r="B12" s="34" t="n"/>
+      <c r="C12" s="33" t="n"/>
+      <c r="D12" s="30" t="n"/>
+      <c r="E12" s="30" t="n"/>
+      <c r="F12" s="30" t="n"/>
+      <c r="G12" s="30" t="n"/>
+      <c r="H12" s="30" t="n"/>
+      <c r="I12" s="30" t="n"/>
+    </row>
+    <row r="13" ht="25" customHeight="1">
+      <c r="A13" s="8" t="inlineStr">
         <is>
           <t>Overall Average:</t>
         </is>
       </c>
-      <c r="B9" s="9">
-        <f>IFERROR(AVERAGEIF(C11:C60,"&gt;0"),"-")</f>
+      <c r="B13" s="9">
+        <f>IFERROR(AVERAGEIF(C15:C64,"&gt;0"),"-")</f>
         <v/>
       </c>
-      <c r="C9" s="18" t="n"/>
-    </row>
-    <row r="10" ht="25" customHeight="1">
-      <c r="A10" s="10" t="inlineStr">
+      <c r="D13" s="30" t="n"/>
+      <c r="E13" s="30" t="n"/>
+      <c r="F13" s="30" t="n"/>
+      <c r="G13" s="30" t="n"/>
+      <c r="H13" s="30" t="n"/>
+      <c r="I13" s="30" t="n"/>
+    </row>
+    <row r="14" ht="25" customHeight="1">
+      <c r="A14" s="10" t="inlineStr">
         <is>
           <t>Test #</t>
         </is>
       </c>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B14" s="10" t="inlineStr">
         <is>
           <t>Question Preview</t>
         </is>
       </c>
-      <c r="C10" s="10" t="inlineStr">
+      <c r="C14" s="35" t="inlineStr">
         <is>
           <t>Score</t>
         </is>
       </c>
-      <c r="D10" s="5" t="n"/>
-      <c r="E10" s="5" t="n"/>
-      <c r="F10" s="5" t="n"/>
-      <c r="G10" s="5" t="n"/>
-      <c r="H10" s="5" t="n"/>
-      <c r="I10" s="5" t="n"/>
-    </row>
-    <row r="11" ht="30" customHeight="1">
-      <c r="A11" s="11" t="n">
+      <c r="D14" s="30" t="n"/>
+      <c r="E14" s="30" t="n"/>
+      <c r="F14" s="30" t="n"/>
+      <c r="G14" s="30" t="n"/>
+      <c r="H14" s="30" t="n"/>
+      <c r="I14" s="30" t="n"/>
+    </row>
+    <row r="15" ht="30" customHeight="1">
+      <c r="A15" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B15" s="12">
         <f>LEFT('1'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C11" s="13">
+      <c r="C15" s="13">
         <f>'1'!H29</f>
         <v/>
       </c>
-      <c r="D11" s="5" t="n"/>
-      <c r="E11" s="5" t="n"/>
-      <c r="F11" s="5" t="n"/>
-      <c r="G11" s="5" t="n"/>
-      <c r="H11" s="5" t="n"/>
-      <c r="I11" s="5" t="n"/>
-    </row>
-    <row r="12" ht="30" customHeight="1">
-      <c r="A12" s="11" t="n">
+      <c r="D15" s="30" t="n"/>
+      <c r="E15" s="30" t="n"/>
+      <c r="F15" s="30" t="n"/>
+      <c r="G15" s="30" t="n"/>
+      <c r="H15" s="30" t="n"/>
+      <c r="I15" s="30" t="n"/>
+    </row>
+    <row r="16" ht="30" customHeight="1">
+      <c r="A16" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B16" s="12">
         <f>LEFT('2'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C12" s="13">
+      <c r="C16" s="13">
         <f>'2'!H29</f>
         <v/>
       </c>
-      <c r="D12" s="5" t="n"/>
-      <c r="E12" s="5" t="n"/>
-      <c r="F12" s="5" t="n"/>
-      <c r="G12" s="5" t="n"/>
-      <c r="H12" s="5" t="n"/>
-      <c r="I12" s="5" t="n"/>
-    </row>
-    <row r="13" ht="30" customHeight="1">
-      <c r="A13" s="11" t="n">
+      <c r="D16" s="30" t="n"/>
+      <c r="E16" s="30" t="n"/>
+      <c r="F16" s="30" t="n"/>
+      <c r="G16" s="30" t="n"/>
+      <c r="H16" s="30" t="n"/>
+      <c r="I16" s="30" t="n"/>
+    </row>
+    <row r="17" ht="30" customHeight="1">
+      <c r="A17" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B17" s="12">
         <f>LEFT('3'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C13" s="13">
+      <c r="C17" s="13">
         <f>'3'!H29</f>
         <v/>
       </c>
-      <c r="D13" s="5" t="n"/>
-      <c r="E13" s="5" t="n"/>
-      <c r="F13" s="5" t="n"/>
-      <c r="G13" s="5" t="n"/>
-      <c r="H13" s="5" t="n"/>
-      <c r="I13" s="5" t="n"/>
-    </row>
-    <row r="14" ht="30" customHeight="1">
-      <c r="A14" s="11" t="n">
+      <c r="D17" s="30" t="n"/>
+      <c r="E17" s="30" t="n"/>
+      <c r="F17" s="30" t="n"/>
+      <c r="G17" s="30" t="n"/>
+      <c r="H17" s="30" t="n"/>
+      <c r="I17" s="30" t="n"/>
+    </row>
+    <row r="18" ht="30" customHeight="1">
+      <c r="A18" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B18" s="12">
         <f>LEFT('4'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C14" s="13">
+      <c r="C18" s="13">
         <f>'4'!H29</f>
         <v/>
       </c>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
-      <c r="I14" s="5" t="n"/>
-    </row>
-    <row r="15" ht="30" customHeight="1">
-      <c r="A15" s="11" t="n">
+      <c r="D18" s="30" t="n"/>
+      <c r="E18" s="30" t="n"/>
+      <c r="F18" s="30" t="n"/>
+      <c r="G18" s="30" t="n"/>
+      <c r="H18" s="30" t="n"/>
+      <c r="I18" s="30" t="n"/>
+    </row>
+    <row r="19" ht="30" customHeight="1">
+      <c r="A19" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B19" s="12">
         <f>LEFT('5'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C15" s="13">
+      <c r="C19" s="13">
         <f>'5'!H29</f>
         <v/>
       </c>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
-      <c r="I15" s="5" t="n"/>
-    </row>
-    <row r="16" ht="30" customHeight="1">
-      <c r="A16" s="11" t="n">
+      <c r="D19" s="30" t="n"/>
+      <c r="E19" s="30" t="n"/>
+      <c r="F19" s="30" t="n"/>
+      <c r="G19" s="30" t="n"/>
+      <c r="H19" s="30" t="n"/>
+      <c r="I19" s="30" t="n"/>
+    </row>
+    <row r="20" ht="30" customHeight="1">
+      <c r="A20" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B20" s="12">
         <f>LEFT('6'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C16" s="13">
+      <c r="C20" s="13">
         <f>'6'!H29</f>
         <v/>
       </c>
-      <c r="D16" s="5" t="n"/>
-      <c r="E16" s="5" t="n"/>
-      <c r="F16" s="5" t="n"/>
-      <c r="G16" s="5" t="n"/>
-      <c r="H16" s="5" t="n"/>
-      <c r="I16" s="5" t="n"/>
-    </row>
-    <row r="17" ht="30" customHeight="1">
-      <c r="A17" s="11" t="n">
+      <c r="D20" s="30" t="n"/>
+      <c r="E20" s="30" t="n"/>
+      <c r="F20" s="30" t="n"/>
+      <c r="G20" s="30" t="n"/>
+      <c r="H20" s="30" t="n"/>
+      <c r="I20" s="30" t="n"/>
+    </row>
+    <row r="21" ht="30" customHeight="1">
+      <c r="A21" s="11" t="n">
         <v>7</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B21" s="12">
         <f>LEFT('7'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C17" s="13">
+      <c r="C21" s="13">
         <f>'7'!H29</f>
-        <v/>
-      </c>
-      <c r="D17" s="5" t="n"/>
-      <c r="E17" s="5" t="n"/>
-      <c r="F17" s="5" t="n"/>
-      <c r="G17" s="5" t="n"/>
-      <c r="H17" s="5" t="n"/>
-      <c r="I17" s="5" t="n"/>
-    </row>
-    <row r="18" ht="30" customHeight="1">
-      <c r="A18" s="11" t="n">
-        <v>8</v>
-      </c>
-      <c r="B18" s="12">
-        <f>LEFT('8'!A4, 200)</f>
-        <v/>
-      </c>
-      <c r="C18" s="13">
-        <f>'8'!H29</f>
-        <v/>
-      </c>
-      <c r="D18" s="5" t="n"/>
-      <c r="E18" s="5" t="n"/>
-      <c r="F18" s="5" t="n"/>
-      <c r="G18" s="5" t="n"/>
-      <c r="H18" s="5" t="n"/>
-      <c r="I18" s="5" t="n"/>
-    </row>
-    <row r="19" ht="30" customHeight="1">
-      <c r="A19" s="11" t="n">
-        <v>9</v>
-      </c>
-      <c r="B19" s="12">
-        <f>LEFT('9'!A4, 200)</f>
-        <v/>
-      </c>
-      <c r="C19" s="13">
-        <f>'9'!H29</f>
-        <v/>
-      </c>
-      <c r="D19" s="5" t="n"/>
-      <c r="E19" s="5" t="n"/>
-      <c r="F19" s="5" t="n"/>
-      <c r="G19" s="5" t="n"/>
-      <c r="H19" s="5" t="n"/>
-      <c r="I19" s="5" t="n"/>
-    </row>
-    <row r="20" ht="30" customHeight="1">
-      <c r="A20" s="11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B20" s="12">
-        <f>LEFT('10'!A4, 200)</f>
-        <v/>
-      </c>
-      <c r="C20" s="13">
-        <f>'10'!H29</f>
-        <v/>
-      </c>
-      <c r="D20" s="5" t="n"/>
-      <c r="E20" s="5" t="n"/>
-      <c r="F20" s="5" t="n"/>
-      <c r="G20" s="5" t="n"/>
-      <c r="H20" s="5" t="n"/>
-      <c r="I20" s="5" t="n"/>
-    </row>
-    <row r="21" ht="30" customHeight="1">
-      <c r="A21" s="11" t="n">
-        <v>11</v>
-      </c>
-      <c r="B21" s="12">
-        <f>LEFT('11'!A4, 200)</f>
-        <v/>
-      </c>
-      <c r="C21" s="13">
-        <f>'11'!H29</f>
         <v/>
       </c>
       <c r="D21" s="5" t="n"/>
@@ -1059,14 +1087,14 @@
     </row>
     <row r="22" ht="30" customHeight="1">
       <c r="A22" s="11" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B22" s="12">
-        <f>LEFT('12'!A4, 200)</f>
+        <f>LEFT('8'!A4, 200)</f>
         <v/>
       </c>
       <c r="C22" s="13">
-        <f>'12'!H29</f>
+        <f>'8'!H29</f>
         <v/>
       </c>
       <c r="D22" s="5" t="n"/>
@@ -1078,14 +1106,14 @@
     </row>
     <row r="23" ht="30" customHeight="1">
       <c r="A23" s="11" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B23" s="12">
-        <f>LEFT('13'!A4, 200)</f>
+        <f>LEFT('9'!A4, 200)</f>
         <v/>
       </c>
       <c r="C23" s="13">
-        <f>'13'!H29</f>
+        <f>'9'!H29</f>
         <v/>
       </c>
       <c r="D23" s="5" t="n"/>
@@ -1097,14 +1125,14 @@
     </row>
     <row r="24" ht="30" customHeight="1">
       <c r="A24" s="11" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B24" s="12">
-        <f>LEFT('14'!A4, 200)</f>
+        <f>LEFT('10'!A4, 200)</f>
         <v/>
       </c>
       <c r="C24" s="13">
-        <f>'14'!H29</f>
+        <f>'10'!H29</f>
         <v/>
       </c>
       <c r="D24" s="5" t="n"/>
@@ -1116,14 +1144,14 @@
     </row>
     <row r="25" ht="30" customHeight="1">
       <c r="A25" s="11" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B25" s="12">
-        <f>LEFT('15'!A4, 200)</f>
+        <f>LEFT('11'!A4, 200)</f>
         <v/>
       </c>
       <c r="C25" s="13">
-        <f>'15'!H29</f>
+        <f>'11'!H29</f>
         <v/>
       </c>
       <c r="D25" s="5" t="n"/>
@@ -1135,14 +1163,14 @@
     </row>
     <row r="26" ht="30" customHeight="1">
       <c r="A26" s="11" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B26" s="12">
-        <f>LEFT('16'!A4, 200)</f>
+        <f>LEFT('12'!A4, 200)</f>
         <v/>
       </c>
       <c r="C26" s="13">
-        <f>'16'!H29</f>
+        <f>'12'!H29</f>
         <v/>
       </c>
       <c r="D26" s="5" t="n"/>
@@ -1154,14 +1182,14 @@
     </row>
     <row r="27" ht="30" customHeight="1">
       <c r="A27" s="11" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B27" s="12">
-        <f>LEFT('17'!A4, 200)</f>
+        <f>LEFT('13'!A4, 200)</f>
         <v/>
       </c>
       <c r="C27" s="13">
-        <f>'17'!H29</f>
+        <f>'13'!H29</f>
         <v/>
       </c>
       <c r="D27" s="5" t="n"/>
@@ -1173,14 +1201,14 @@
     </row>
     <row r="28" ht="30" customHeight="1">
       <c r="A28" s="11" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B28" s="12">
-        <f>LEFT('18'!A4, 200)</f>
+        <f>LEFT('14'!A4, 200)</f>
         <v/>
       </c>
       <c r="C28" s="13">
-        <f>'18'!H29</f>
+        <f>'14'!H29</f>
         <v/>
       </c>
       <c r="D28" s="5" t="n"/>
@@ -1192,14 +1220,14 @@
     </row>
     <row r="29" ht="30" customHeight="1">
       <c r="A29" s="11" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B29" s="12">
-        <f>LEFT('19'!A4, 200)</f>
+        <f>LEFT('15'!A4, 200)</f>
         <v/>
       </c>
       <c r="C29" s="13">
-        <f>'19'!H29</f>
+        <f>'15'!H29</f>
         <v/>
       </c>
       <c r="D29" s="5" t="n"/>
@@ -1211,14 +1239,14 @@
     </row>
     <row r="30" ht="30" customHeight="1">
       <c r="A30" s="11" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B30" s="12">
-        <f>LEFT('20'!A4, 200)</f>
+        <f>LEFT('16'!A4, 200)</f>
         <v/>
       </c>
       <c r="C30" s="13">
-        <f>'20'!H29</f>
+        <f>'16'!H29</f>
         <v/>
       </c>
       <c r="D30" s="5" t="n"/>
@@ -1230,14 +1258,14 @@
     </row>
     <row r="31" ht="30" customHeight="1">
       <c r="A31" s="11" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B31" s="12">
-        <f>LEFT('21'!A4, 200)</f>
+        <f>LEFT('17'!A4, 200)</f>
         <v/>
       </c>
       <c r="C31" s="13">
-        <f>'21'!H29</f>
+        <f>'17'!H29</f>
         <v/>
       </c>
       <c r="D31" s="5" t="n"/>
@@ -1249,14 +1277,14 @@
     </row>
     <row r="32" ht="30" customHeight="1">
       <c r="A32" s="11" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B32" s="12">
-        <f>LEFT('22'!A4, 200)</f>
+        <f>LEFT('18'!A4, 200)</f>
         <v/>
       </c>
       <c r="C32" s="13">
-        <f>'22'!H29</f>
+        <f>'18'!H29</f>
         <v/>
       </c>
       <c r="D32" s="5" t="n"/>
@@ -1268,14 +1296,14 @@
     </row>
     <row r="33" ht="30" customHeight="1">
       <c r="A33" s="11" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B33" s="12">
-        <f>LEFT('23'!A4, 200)</f>
+        <f>LEFT('19'!A4, 200)</f>
         <v/>
       </c>
       <c r="C33" s="13">
-        <f>'23'!H29</f>
+        <f>'19'!H29</f>
         <v/>
       </c>
       <c r="D33" s="5" t="n"/>
@@ -1287,14 +1315,14 @@
     </row>
     <row r="34" ht="30" customHeight="1">
       <c r="A34" s="11" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B34" s="12">
-        <f>LEFT('24'!A4, 200)</f>
+        <f>LEFT('20'!A4, 200)</f>
         <v/>
       </c>
       <c r="C34" s="13">
-        <f>'24'!H29</f>
+        <f>'20'!H29</f>
         <v/>
       </c>
       <c r="D34" s="5" t="n"/>
@@ -1306,14 +1334,14 @@
     </row>
     <row r="35" ht="30" customHeight="1">
       <c r="A35" s="11" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B35" s="12">
-        <f>LEFT('25'!A4, 200)</f>
+        <f>LEFT('21'!A4, 200)</f>
         <v/>
       </c>
       <c r="C35" s="13">
-        <f>'25'!H29</f>
+        <f>'21'!H29</f>
         <v/>
       </c>
       <c r="D35" s="5" t="n"/>
@@ -1325,14 +1353,14 @@
     </row>
     <row r="36" ht="30" customHeight="1">
       <c r="A36" s="11" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B36" s="12">
-        <f>LEFT('26'!A4, 200)</f>
+        <f>LEFT('22'!A4, 200)</f>
         <v/>
       </c>
       <c r="C36" s="13">
-        <f>'26'!H29</f>
+        <f>'22'!H29</f>
         <v/>
       </c>
       <c r="D36" s="5" t="n"/>
@@ -1344,14 +1372,14 @@
     </row>
     <row r="37" ht="30" customHeight="1">
       <c r="A37" s="11" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B37" s="12">
-        <f>LEFT('27'!A4, 200)</f>
+        <f>LEFT('23'!A4, 200)</f>
         <v/>
       </c>
       <c r="C37" s="13">
-        <f>'27'!H29</f>
+        <f>'23'!H29</f>
         <v/>
       </c>
       <c r="D37" s="5" t="n"/>
@@ -1363,14 +1391,14 @@
     </row>
     <row r="38" ht="30" customHeight="1">
       <c r="A38" s="11" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B38" s="12">
-        <f>LEFT('28'!A4, 200)</f>
+        <f>LEFT('24'!A4, 200)</f>
         <v/>
       </c>
       <c r="C38" s="13">
-        <f>'28'!H29</f>
+        <f>'24'!H29</f>
         <v/>
       </c>
       <c r="D38" s="5" t="n"/>
@@ -1382,14 +1410,14 @@
     </row>
     <row r="39" ht="30" customHeight="1">
       <c r="A39" s="11" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B39" s="12">
-        <f>LEFT('29'!A4, 200)</f>
+        <f>LEFT('25'!A4, 200)</f>
         <v/>
       </c>
       <c r="C39" s="13">
-        <f>'29'!H29</f>
+        <f>'25'!H29</f>
         <v/>
       </c>
       <c r="D39" s="5" t="n"/>
@@ -1401,14 +1429,14 @@
     </row>
     <row r="40" ht="30" customHeight="1">
       <c r="A40" s="11" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B40" s="12">
-        <f>LEFT('30'!A4, 200)</f>
+        <f>LEFT('26'!A4, 200)</f>
         <v/>
       </c>
       <c r="C40" s="13">
-        <f>'30'!H29</f>
+        <f>'26'!H29</f>
         <v/>
       </c>
       <c r="D40" s="5" t="n"/>
@@ -1420,14 +1448,14 @@
     </row>
     <row r="41" ht="30" customHeight="1">
       <c r="A41" s="11" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B41" s="12">
-        <f>LEFT('31'!A4, 200)</f>
+        <f>LEFT('27'!A4, 200)</f>
         <v/>
       </c>
       <c r="C41" s="13">
-        <f>'31'!H29</f>
+        <f>'27'!H29</f>
         <v/>
       </c>
       <c r="D41" s="5" t="n"/>
@@ -1439,14 +1467,14 @@
     </row>
     <row r="42" ht="30" customHeight="1">
       <c r="A42" s="11" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B42" s="12">
-        <f>LEFT('32'!A4, 200)</f>
+        <f>LEFT('28'!A4, 200)</f>
         <v/>
       </c>
       <c r="C42" s="13">
-        <f>'32'!H29</f>
+        <f>'28'!H29</f>
         <v/>
       </c>
       <c r="D42" s="5" t="n"/>
@@ -1458,14 +1486,14 @@
     </row>
     <row r="43" ht="30" customHeight="1">
       <c r="A43" s="11" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B43" s="12">
-        <f>LEFT('33'!A4, 200)</f>
+        <f>LEFT('29'!A4, 200)</f>
         <v/>
       </c>
       <c r="C43" s="13">
-        <f>'33'!H29</f>
+        <f>'29'!H29</f>
         <v/>
       </c>
       <c r="D43" s="5" t="n"/>
@@ -1477,14 +1505,14 @@
     </row>
     <row r="44" ht="30" customHeight="1">
       <c r="A44" s="11" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B44" s="12">
-        <f>LEFT('34'!A4, 200)</f>
+        <f>LEFT('30'!A4, 200)</f>
         <v/>
       </c>
       <c r="C44" s="13">
-        <f>'34'!H29</f>
+        <f>'30'!H29</f>
         <v/>
       </c>
       <c r="D44" s="5" t="n"/>
@@ -1496,14 +1524,14 @@
     </row>
     <row r="45" ht="30" customHeight="1">
       <c r="A45" s="11" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B45" s="12">
-        <f>LEFT('35'!A4, 200)</f>
+        <f>LEFT('31'!A4, 200)</f>
         <v/>
       </c>
       <c r="C45" s="13">
-        <f>'35'!H29</f>
+        <f>'31'!H29</f>
         <v/>
       </c>
       <c r="D45" s="5" t="n"/>
@@ -1515,14 +1543,14 @@
     </row>
     <row r="46" ht="30" customHeight="1">
       <c r="A46" s="11" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B46" s="12">
-        <f>LEFT('36'!A4, 200)</f>
+        <f>LEFT('32'!A4, 200)</f>
         <v/>
       </c>
       <c r="C46" s="13">
-        <f>'36'!H29</f>
+        <f>'32'!H29</f>
         <v/>
       </c>
       <c r="D46" s="5" t="n"/>
@@ -1534,14 +1562,14 @@
     </row>
     <row r="47" ht="30" customHeight="1">
       <c r="A47" s="11" t="n">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B47" s="12">
-        <f>LEFT('37'!A4, 200)</f>
+        <f>LEFT('33'!A4, 200)</f>
         <v/>
       </c>
       <c r="C47" s="13">
-        <f>'37'!H29</f>
+        <f>'33'!H29</f>
         <v/>
       </c>
       <c r="D47" s="5" t="n"/>
@@ -1553,14 +1581,14 @@
     </row>
     <row r="48" ht="30" customHeight="1">
       <c r="A48" s="11" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B48" s="12">
-        <f>LEFT('38'!A4, 200)</f>
+        <f>LEFT('34'!A4, 200)</f>
         <v/>
       </c>
       <c r="C48" s="13">
-        <f>'38'!H29</f>
+        <f>'34'!H29</f>
         <v/>
       </c>
       <c r="D48" s="5" t="n"/>
@@ -1572,14 +1600,14 @@
     </row>
     <row r="49" ht="30" customHeight="1">
       <c r="A49" s="11" t="n">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B49" s="12">
-        <f>LEFT('39'!A4, 200)</f>
+        <f>LEFT('35'!A4, 200)</f>
         <v/>
       </c>
       <c r="C49" s="13">
-        <f>'39'!H29</f>
+        <f>'35'!H29</f>
         <v/>
       </c>
       <c r="D49" s="5" t="n"/>
@@ -1591,14 +1619,14 @@
     </row>
     <row r="50" ht="30" customHeight="1">
       <c r="A50" s="11" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B50" s="12">
-        <f>LEFT('40'!A4, 200)</f>
+        <f>LEFT('36'!A4, 200)</f>
         <v/>
       </c>
       <c r="C50" s="13">
-        <f>'40'!H29</f>
+        <f>'36'!H29</f>
         <v/>
       </c>
       <c r="D50" s="5" t="n"/>
@@ -1610,14 +1638,14 @@
     </row>
     <row r="51" ht="30" customHeight="1">
       <c r="A51" s="11" t="n">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B51" s="12">
-        <f>LEFT('41'!A4, 200)</f>
+        <f>LEFT('37'!A4, 200)</f>
         <v/>
       </c>
       <c r="C51" s="13">
-        <f>'41'!H29</f>
+        <f>'37'!H29</f>
         <v/>
       </c>
       <c r="D51" s="5" t="n"/>
@@ -1629,14 +1657,14 @@
     </row>
     <row r="52" ht="30" customHeight="1">
       <c r="A52" s="11" t="n">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B52" s="12">
-        <f>LEFT('42'!A4, 200)</f>
+        <f>LEFT('38'!A4, 200)</f>
         <v/>
       </c>
       <c r="C52" s="13">
-        <f>'42'!H29</f>
+        <f>'38'!H29</f>
         <v/>
       </c>
       <c r="D52" s="5" t="n"/>
@@ -1648,14 +1676,14 @@
     </row>
     <row r="53" ht="30" customHeight="1">
       <c r="A53" s="11" t="n">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B53" s="12">
-        <f>LEFT('43'!A4, 200)</f>
+        <f>LEFT('39'!A4, 200)</f>
         <v/>
       </c>
       <c r="C53" s="13">
-        <f>'43'!H29</f>
+        <f>'39'!H29</f>
         <v/>
       </c>
       <c r="D53" s="5" t="n"/>
@@ -1667,14 +1695,14 @@
     </row>
     <row r="54" ht="30" customHeight="1">
       <c r="A54" s="11" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B54" s="12">
-        <f>LEFT('44'!A4, 200)</f>
+        <f>LEFT('40'!A4, 200)</f>
         <v/>
       </c>
       <c r="C54" s="13">
-        <f>'44'!H29</f>
+        <f>'40'!H29</f>
         <v/>
       </c>
       <c r="D54" s="5" t="n"/>
@@ -1686,14 +1714,14 @@
     </row>
     <row r="55" ht="30" customHeight="1">
       <c r="A55" s="11" t="n">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B55" s="12">
-        <f>LEFT('45'!A4, 200)</f>
+        <f>LEFT('41'!A4, 200)</f>
         <v/>
       </c>
       <c r="C55" s="13">
-        <f>'45'!H29</f>
+        <f>'41'!H29</f>
         <v/>
       </c>
       <c r="D55" s="5" t="n"/>
@@ -1705,14 +1733,14 @@
     </row>
     <row r="56" ht="30" customHeight="1">
       <c r="A56" s="11" t="n">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B56" s="12">
-        <f>LEFT('46'!A4, 200)</f>
+        <f>LEFT('42'!A4, 200)</f>
         <v/>
       </c>
       <c r="C56" s="13">
-        <f>'46'!H29</f>
+        <f>'42'!H29</f>
         <v/>
       </c>
       <c r="D56" s="5" t="n"/>
@@ -1724,14 +1752,14 @@
     </row>
     <row r="57" ht="30" customHeight="1">
       <c r="A57" s="11" t="n">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B57" s="12">
-        <f>LEFT('47'!A4, 200)</f>
+        <f>LEFT('43'!A4, 200)</f>
         <v/>
       </c>
       <c r="C57" s="13">
-        <f>'47'!H29</f>
+        <f>'43'!H29</f>
         <v/>
       </c>
       <c r="D57" s="5" t="n"/>
@@ -1743,14 +1771,14 @@
     </row>
     <row r="58" ht="30" customHeight="1">
       <c r="A58" s="11" t="n">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B58" s="12">
-        <f>LEFT('48'!A4, 200)</f>
+        <f>LEFT('44'!A4, 200)</f>
         <v/>
       </c>
       <c r="C58" s="13">
-        <f>'48'!H29</f>
+        <f>'44'!H29</f>
         <v/>
       </c>
       <c r="D58" s="5" t="n"/>
@@ -1762,14 +1790,14 @@
     </row>
     <row r="59" ht="30" customHeight="1">
       <c r="A59" s="11" t="n">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B59" s="12">
-        <f>LEFT('49'!A4, 200)</f>
+        <f>LEFT('45'!A4, 200)</f>
         <v/>
       </c>
       <c r="C59" s="13">
-        <f>'49'!H29</f>
+        <f>'45'!H29</f>
         <v/>
       </c>
       <c r="D59" s="5" t="n"/>
@@ -1781,14 +1809,14 @@
     </row>
     <row r="60" ht="30" customHeight="1">
       <c r="A60" s="11" t="n">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B60" s="12">
-        <f>LEFT('50'!A4, 200)</f>
+        <f>LEFT('46'!A4, 200)</f>
         <v/>
       </c>
       <c r="C60" s="13">
-        <f>'50'!H29</f>
+        <f>'46'!H29</f>
         <v/>
       </c>
       <c r="D60" s="5" t="n"/>
@@ -1798,19 +1826,73 @@
       <c r="H60" s="5" t="n"/>
       <c r="I60" s="5" t="n"/>
     </row>
+    <row r="61" ht="30" customHeight="1">
+      <c r="A61" s="11" t="n">
+        <v>47</v>
+      </c>
+      <c r="B61" s="12">
+        <f>LEFT('47'!A4, 200)</f>
+        <v/>
+      </c>
+      <c r="C61" s="13">
+        <f>'47'!H29</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" ht="30" customHeight="1">
+      <c r="A62" s="11" t="n">
+        <v>48</v>
+      </c>
+      <c r="B62" s="12">
+        <f>LEFT('48'!A4, 200)</f>
+        <v/>
+      </c>
+      <c r="C62" s="13">
+        <f>'48'!H29</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" ht="30" customHeight="1">
+      <c r="A63" s="11" t="n">
+        <v>49</v>
+      </c>
+      <c r="B63" s="12">
+        <f>LEFT('49'!A4, 200)</f>
+        <v/>
+      </c>
+      <c r="C63" s="13">
+        <f>'49'!H29</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" ht="30" customHeight="1">
+      <c r="A64" s="11" t="n">
+        <v>50</v>
+      </c>
+      <c r="B64" s="12">
+        <f>LEFT('50'!A4, 200)</f>
+        <v/>
+      </c>
+      <c r="C64" s="13">
+        <f>'50'!H29</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B10"/>
-    <mergeCell ref="B9:C9"/>
+  <mergeCells count="4">
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation sqref="D7:I7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select ✓ or X" promptTitle="Database Selection" prompt="Click to select ✓ or X" type="list">
       <formula1>"✓,X"</formula1>
     </dataValidation>
     <dataValidation sqref="A7:F7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select ✓ or X" promptTitle="Database Selection" prompt="Click to select ✓ or X" type="list">
+      <formula1>"✓,X"</formula1>
+    </dataValidation>
+    <dataValidation sqref="B6:B11" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select ✓ or X" promptTitle="Database Selection" prompt="Click to select ✓ or X" type="list">
       <formula1>"✓,X"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Complete formatting overhaul: fix alignment and add percentage
Comprehensive formatting improvements:
- Optimized column widths (A=20, B=50, C=12) for better proportions
- Fixed all database checkbox cell borders and fills
- Enhanced overall average display:
  * Column B: Score with " / 10" format (e.g., "8.50 / 10")
  * Column C: Percentage format (e.g., "85%")
- Verified and corrected all cell borders, fills, fonts, alignments
- Consistent white backgrounds for data cells
- Clean visual hierarchy throughout

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/user_testing_template.xlsx
+++ b/user_testing_template.xlsx
@@ -66,8 +66,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.00&quot; / 10&quot;"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -278,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -359,6 +360,31 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -734,8 +760,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10" customWidth="1" min="1" max="1"/>
-    <col width="60" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="50" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
@@ -751,6 +777,8 @@
           <t>AEGIS Performance Testing - Summary</t>
         </is>
       </c>
+      <c r="B1" s="17" t="n"/>
+      <c r="C1" s="18" t="n"/>
       <c r="D1" s="30" t="n"/>
       <c r="E1" s="30" t="n"/>
       <c r="F1" s="30" t="n"/>
@@ -775,11 +803,12 @@
           <t>Testing Description:</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" s="36" t="inlineStr">
         <is>
           <t>Enter overall testing description here (e.g., Testing for Q3 earnings, Testing RTS functionality, etc.)</t>
         </is>
       </c>
+      <c r="C3" s="18" t="n"/>
       <c r="D3" s="30" t="n"/>
       <c r="E3" s="30" t="n"/>
       <c r="F3" s="30" t="n"/>
@@ -804,6 +833,8 @@
           <t>Database Selection (applies to all tests)</t>
         </is>
       </c>
+      <c r="B5" s="17" t="n"/>
+      <c r="C5" s="18" t="n"/>
       <c r="D5" s="30" t="n"/>
       <c r="E5" s="30" t="n"/>
       <c r="F5" s="30" t="n"/>
@@ -818,7 +849,7 @@
         </is>
       </c>
       <c r="B6" s="31" t="inlineStr"/>
-      <c r="C6" s="28" t="n"/>
+      <c r="C6" s="37" t="n"/>
       <c r="D6" s="28" t="n"/>
       <c r="E6" s="28" t="n"/>
       <c r="F6" s="28" t="n"/>
@@ -833,7 +864,7 @@
         </is>
       </c>
       <c r="B7" s="31" t="inlineStr"/>
-      <c r="C7" s="28" t="n"/>
+      <c r="C7" s="37" t="n"/>
       <c r="D7" s="28" t="n"/>
       <c r="E7" s="28" t="n"/>
       <c r="F7" s="28" t="n"/>
@@ -848,7 +879,7 @@
         </is>
       </c>
       <c r="B8" s="31" t="inlineStr"/>
-      <c r="C8" s="30" t="n"/>
+      <c r="C8" s="38" t="n"/>
       <c r="D8" s="30" t="n"/>
       <c r="E8" s="30" t="n"/>
       <c r="F8" s="30" t="n"/>
@@ -863,7 +894,7 @@
         </is>
       </c>
       <c r="B9" s="32" t="inlineStr"/>
-      <c r="C9" s="30" t="n"/>
+      <c r="C9" s="38" t="n"/>
       <c r="D9" s="30" t="n"/>
       <c r="E9" s="30" t="n"/>
       <c r="F9" s="30" t="n"/>
@@ -878,7 +909,7 @@
         </is>
       </c>
       <c r="B10" s="31" t="inlineStr"/>
-      <c r="C10" s="28" t="n"/>
+      <c r="C10" s="37" t="n"/>
       <c r="D10" s="30" t="n"/>
       <c r="E10" s="30" t="n"/>
       <c r="F10" s="30" t="n"/>
@@ -893,7 +924,7 @@
         </is>
       </c>
       <c r="B11" s="31" t="inlineStr"/>
-      <c r="C11" s="33" t="n"/>
+      <c r="C11" s="39" t="n"/>
       <c r="D11" s="30" t="n"/>
       <c r="E11" s="30" t="n"/>
       <c r="F11" s="30" t="n"/>
@@ -918,8 +949,12 @@
           <t>Overall Average:</t>
         </is>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="40">
         <f>IFERROR(AVERAGEIF(C15:C64,"&gt;0"),"-")</f>
+        <v/>
+      </c>
+      <c r="C13" s="41">
+        <f>IFERROR(AVERAGEIF(C15:C64,"&gt;0")/10,"-")</f>
         <v/>
       </c>
       <c r="D13" s="30" t="n"/>
@@ -953,14 +988,14 @@
       <c r="I14" s="30" t="n"/>
     </row>
     <row r="15" ht="30" customHeight="1">
-      <c r="A15" s="11" t="n">
+      <c r="A15" s="42" t="n">
         <v>1</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="43">
         <f>LEFT('1'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="44">
         <f>'1'!H29</f>
         <v/>
       </c>
@@ -972,14 +1007,14 @@
       <c r="I15" s="30" t="n"/>
     </row>
     <row r="16" ht="30" customHeight="1">
-      <c r="A16" s="11" t="n">
+      <c r="A16" s="42" t="n">
         <v>2</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="43">
         <f>LEFT('2'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="44">
         <f>'2'!H29</f>
         <v/>
       </c>
@@ -991,14 +1026,14 @@
       <c r="I16" s="30" t="n"/>
     </row>
     <row r="17" ht="30" customHeight="1">
-      <c r="A17" s="11" t="n">
+      <c r="A17" s="42" t="n">
         <v>3</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="43">
         <f>LEFT('3'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="44">
         <f>'3'!H29</f>
         <v/>
       </c>
@@ -1010,14 +1045,14 @@
       <c r="I17" s="30" t="n"/>
     </row>
     <row r="18" ht="30" customHeight="1">
-      <c r="A18" s="11" t="n">
+      <c r="A18" s="42" t="n">
         <v>4</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="43">
         <f>LEFT('4'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="44">
         <f>'4'!H29</f>
         <v/>
       </c>
@@ -1029,14 +1064,14 @@
       <c r="I18" s="30" t="n"/>
     </row>
     <row r="19" ht="30" customHeight="1">
-      <c r="A19" s="11" t="n">
+      <c r="A19" s="42" t="n">
         <v>5</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="43">
         <f>LEFT('5'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="44">
         <f>'5'!H29</f>
         <v/>
       </c>
@@ -1048,14 +1083,14 @@
       <c r="I19" s="30" t="n"/>
     </row>
     <row r="20" ht="30" customHeight="1">
-      <c r="A20" s="11" t="n">
+      <c r="A20" s="42" t="n">
         <v>6</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="43">
         <f>LEFT('6'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="44">
         <f>'6'!H29</f>
         <v/>
       </c>
@@ -1067,14 +1102,14 @@
       <c r="I20" s="30" t="n"/>
     </row>
     <row r="21" ht="30" customHeight="1">
-      <c r="A21" s="11" t="n">
+      <c r="A21" s="42" t="n">
         <v>7</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="43">
         <f>LEFT('7'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="44">
         <f>'7'!H29</f>
         <v/>
       </c>
@@ -1086,14 +1121,14 @@
       <c r="I21" s="5" t="n"/>
     </row>
     <row r="22" ht="30" customHeight="1">
-      <c r="A22" s="11" t="n">
+      <c r="A22" s="42" t="n">
         <v>8</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="43">
         <f>LEFT('8'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="44">
         <f>'8'!H29</f>
         <v/>
       </c>
@@ -1105,14 +1140,14 @@
       <c r="I22" s="5" t="n"/>
     </row>
     <row r="23" ht="30" customHeight="1">
-      <c r="A23" s="11" t="n">
+      <c r="A23" s="42" t="n">
         <v>9</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="43">
         <f>LEFT('9'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="44">
         <f>'9'!H29</f>
         <v/>
       </c>
@@ -1124,14 +1159,14 @@
       <c r="I23" s="5" t="n"/>
     </row>
     <row r="24" ht="30" customHeight="1">
-      <c r="A24" s="11" t="n">
+      <c r="A24" s="42" t="n">
         <v>10</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="43">
         <f>LEFT('10'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="44">
         <f>'10'!H29</f>
         <v/>
       </c>
@@ -1143,14 +1178,14 @@
       <c r="I24" s="5" t="n"/>
     </row>
     <row r="25" ht="30" customHeight="1">
-      <c r="A25" s="11" t="n">
+      <c r="A25" s="42" t="n">
         <v>11</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="43">
         <f>LEFT('11'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C25" s="13">
+      <c r="C25" s="44">
         <f>'11'!H29</f>
         <v/>
       </c>
@@ -1162,14 +1197,14 @@
       <c r="I25" s="5" t="n"/>
     </row>
     <row r="26" ht="30" customHeight="1">
-      <c r="A26" s="11" t="n">
+      <c r="A26" s="42" t="n">
         <v>12</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="43">
         <f>LEFT('12'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="44">
         <f>'12'!H29</f>
         <v/>
       </c>
@@ -1181,14 +1216,14 @@
       <c r="I26" s="5" t="n"/>
     </row>
     <row r="27" ht="30" customHeight="1">
-      <c r="A27" s="11" t="n">
+      <c r="A27" s="42" t="n">
         <v>13</v>
       </c>
-      <c r="B27" s="12">
+      <c r="B27" s="43">
         <f>LEFT('13'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C27" s="13">
+      <c r="C27" s="44">
         <f>'13'!H29</f>
         <v/>
       </c>
@@ -1200,14 +1235,14 @@
       <c r="I27" s="5" t="n"/>
     </row>
     <row r="28" ht="30" customHeight="1">
-      <c r="A28" s="11" t="n">
+      <c r="A28" s="42" t="n">
         <v>14</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="43">
         <f>LEFT('14'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C28" s="13">
+      <c r="C28" s="44">
         <f>'14'!H29</f>
         <v/>
       </c>
@@ -1219,14 +1254,14 @@
       <c r="I28" s="5" t="n"/>
     </row>
     <row r="29" ht="30" customHeight="1">
-      <c r="A29" s="11" t="n">
+      <c r="A29" s="42" t="n">
         <v>15</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29" s="43">
         <f>LEFT('15'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C29" s="13">
+      <c r="C29" s="44">
         <f>'15'!H29</f>
         <v/>
       </c>
@@ -1238,14 +1273,14 @@
       <c r="I29" s="5" t="n"/>
     </row>
     <row r="30" ht="30" customHeight="1">
-      <c r="A30" s="11" t="n">
+      <c r="A30" s="42" t="n">
         <v>16</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B30" s="43">
         <f>LEFT('16'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C30" s="13">
+      <c r="C30" s="44">
         <f>'16'!H29</f>
         <v/>
       </c>
@@ -1257,14 +1292,14 @@
       <c r="I30" s="5" t="n"/>
     </row>
     <row r="31" ht="30" customHeight="1">
-      <c r="A31" s="11" t="n">
+      <c r="A31" s="42" t="n">
         <v>17</v>
       </c>
-      <c r="B31" s="12">
+      <c r="B31" s="43">
         <f>LEFT('17'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C31" s="13">
+      <c r="C31" s="44">
         <f>'17'!H29</f>
         <v/>
       </c>
@@ -1276,14 +1311,14 @@
       <c r="I31" s="5" t="n"/>
     </row>
     <row r="32" ht="30" customHeight="1">
-      <c r="A32" s="11" t="n">
+      <c r="A32" s="42" t="n">
         <v>18</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B32" s="43">
         <f>LEFT('18'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C32" s="13">
+      <c r="C32" s="44">
         <f>'18'!H29</f>
         <v/>
       </c>
@@ -1295,14 +1330,14 @@
       <c r="I32" s="5" t="n"/>
     </row>
     <row r="33" ht="30" customHeight="1">
-      <c r="A33" s="11" t="n">
+      <c r="A33" s="42" t="n">
         <v>19</v>
       </c>
-      <c r="B33" s="12">
+      <c r="B33" s="43">
         <f>LEFT('19'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C33" s="13">
+      <c r="C33" s="44">
         <f>'19'!H29</f>
         <v/>
       </c>
@@ -1314,14 +1349,14 @@
       <c r="I33" s="5" t="n"/>
     </row>
     <row r="34" ht="30" customHeight="1">
-      <c r="A34" s="11" t="n">
+      <c r="A34" s="42" t="n">
         <v>20</v>
       </c>
-      <c r="B34" s="12">
+      <c r="B34" s="43">
         <f>LEFT('20'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C34" s="13">
+      <c r="C34" s="44">
         <f>'20'!H29</f>
         <v/>
       </c>
@@ -1333,14 +1368,14 @@
       <c r="I34" s="5" t="n"/>
     </row>
     <row r="35" ht="30" customHeight="1">
-      <c r="A35" s="11" t="n">
+      <c r="A35" s="42" t="n">
         <v>21</v>
       </c>
-      <c r="B35" s="12">
+      <c r="B35" s="43">
         <f>LEFT('21'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C35" s="13">
+      <c r="C35" s="44">
         <f>'21'!H29</f>
         <v/>
       </c>
@@ -1352,14 +1387,14 @@
       <c r="I35" s="5" t="n"/>
     </row>
     <row r="36" ht="30" customHeight="1">
-      <c r="A36" s="11" t="n">
+      <c r="A36" s="42" t="n">
         <v>22</v>
       </c>
-      <c r="B36" s="12">
+      <c r="B36" s="43">
         <f>LEFT('22'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C36" s="13">
+      <c r="C36" s="44">
         <f>'22'!H29</f>
         <v/>
       </c>
@@ -1371,14 +1406,14 @@
       <c r="I36" s="5" t="n"/>
     </row>
     <row r="37" ht="30" customHeight="1">
-      <c r="A37" s="11" t="n">
+      <c r="A37" s="42" t="n">
         <v>23</v>
       </c>
-      <c r="B37" s="12">
+      <c r="B37" s="43">
         <f>LEFT('23'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C37" s="13">
+      <c r="C37" s="44">
         <f>'23'!H29</f>
         <v/>
       </c>
@@ -1390,14 +1425,14 @@
       <c r="I37" s="5" t="n"/>
     </row>
     <row r="38" ht="30" customHeight="1">
-      <c r="A38" s="11" t="n">
+      <c r="A38" s="42" t="n">
         <v>24</v>
       </c>
-      <c r="B38" s="12">
+      <c r="B38" s="43">
         <f>LEFT('24'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C38" s="13">
+      <c r="C38" s="44">
         <f>'24'!H29</f>
         <v/>
       </c>
@@ -1409,14 +1444,14 @@
       <c r="I38" s="5" t="n"/>
     </row>
     <row r="39" ht="30" customHeight="1">
-      <c r="A39" s="11" t="n">
+      <c r="A39" s="42" t="n">
         <v>25</v>
       </c>
-      <c r="B39" s="12">
+      <c r="B39" s="43">
         <f>LEFT('25'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C39" s="13">
+      <c r="C39" s="44">
         <f>'25'!H29</f>
         <v/>
       </c>
@@ -1428,14 +1463,14 @@
       <c r="I39" s="5" t="n"/>
     </row>
     <row r="40" ht="30" customHeight="1">
-      <c r="A40" s="11" t="n">
+      <c r="A40" s="42" t="n">
         <v>26</v>
       </c>
-      <c r="B40" s="12">
+      <c r="B40" s="43">
         <f>LEFT('26'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C40" s="13">
+      <c r="C40" s="44">
         <f>'26'!H29</f>
         <v/>
       </c>
@@ -1447,14 +1482,14 @@
       <c r="I40" s="5" t="n"/>
     </row>
     <row r="41" ht="30" customHeight="1">
-      <c r="A41" s="11" t="n">
+      <c r="A41" s="42" t="n">
         <v>27</v>
       </c>
-      <c r="B41" s="12">
+      <c r="B41" s="43">
         <f>LEFT('27'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C41" s="13">
+      <c r="C41" s="44">
         <f>'27'!H29</f>
         <v/>
       </c>
@@ -1466,14 +1501,14 @@
       <c r="I41" s="5" t="n"/>
     </row>
     <row r="42" ht="30" customHeight="1">
-      <c r="A42" s="11" t="n">
+      <c r="A42" s="42" t="n">
         <v>28</v>
       </c>
-      <c r="B42" s="12">
+      <c r="B42" s="43">
         <f>LEFT('28'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C42" s="13">
+      <c r="C42" s="44">
         <f>'28'!H29</f>
         <v/>
       </c>
@@ -1485,14 +1520,14 @@
       <c r="I42" s="5" t="n"/>
     </row>
     <row r="43" ht="30" customHeight="1">
-      <c r="A43" s="11" t="n">
+      <c r="A43" s="42" t="n">
         <v>29</v>
       </c>
-      <c r="B43" s="12">
+      <c r="B43" s="43">
         <f>LEFT('29'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C43" s="13">
+      <c r="C43" s="44">
         <f>'29'!H29</f>
         <v/>
       </c>
@@ -1504,14 +1539,14 @@
       <c r="I43" s="5" t="n"/>
     </row>
     <row r="44" ht="30" customHeight="1">
-      <c r="A44" s="11" t="n">
+      <c r="A44" s="42" t="n">
         <v>30</v>
       </c>
-      <c r="B44" s="12">
+      <c r="B44" s="43">
         <f>LEFT('30'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C44" s="13">
+      <c r="C44" s="44">
         <f>'30'!H29</f>
         <v/>
       </c>
@@ -1523,14 +1558,14 @@
       <c r="I44" s="5" t="n"/>
     </row>
     <row r="45" ht="30" customHeight="1">
-      <c r="A45" s="11" t="n">
+      <c r="A45" s="42" t="n">
         <v>31</v>
       </c>
-      <c r="B45" s="12">
+      <c r="B45" s="43">
         <f>LEFT('31'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C45" s="13">
+      <c r="C45" s="44">
         <f>'31'!H29</f>
         <v/>
       </c>
@@ -1542,14 +1577,14 @@
       <c r="I45" s="5" t="n"/>
     </row>
     <row r="46" ht="30" customHeight="1">
-      <c r="A46" s="11" t="n">
+      <c r="A46" s="42" t="n">
         <v>32</v>
       </c>
-      <c r="B46" s="12">
+      <c r="B46" s="43">
         <f>LEFT('32'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C46" s="13">
+      <c r="C46" s="44">
         <f>'32'!H29</f>
         <v/>
       </c>
@@ -1561,14 +1596,14 @@
       <c r="I46" s="5" t="n"/>
     </row>
     <row r="47" ht="30" customHeight="1">
-      <c r="A47" s="11" t="n">
+      <c r="A47" s="42" t="n">
         <v>33</v>
       </c>
-      <c r="B47" s="12">
+      <c r="B47" s="43">
         <f>LEFT('33'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C47" s="13">
+      <c r="C47" s="44">
         <f>'33'!H29</f>
         <v/>
       </c>
@@ -1580,14 +1615,14 @@
       <c r="I47" s="5" t="n"/>
     </row>
     <row r="48" ht="30" customHeight="1">
-      <c r="A48" s="11" t="n">
+      <c r="A48" s="42" t="n">
         <v>34</v>
       </c>
-      <c r="B48" s="12">
+      <c r="B48" s="43">
         <f>LEFT('34'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C48" s="13">
+      <c r="C48" s="44">
         <f>'34'!H29</f>
         <v/>
       </c>
@@ -1599,14 +1634,14 @@
       <c r="I48" s="5" t="n"/>
     </row>
     <row r="49" ht="30" customHeight="1">
-      <c r="A49" s="11" t="n">
+      <c r="A49" s="42" t="n">
         <v>35</v>
       </c>
-      <c r="B49" s="12">
+      <c r="B49" s="43">
         <f>LEFT('35'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C49" s="13">
+      <c r="C49" s="44">
         <f>'35'!H29</f>
         <v/>
       </c>
@@ -1618,14 +1653,14 @@
       <c r="I49" s="5" t="n"/>
     </row>
     <row r="50" ht="30" customHeight="1">
-      <c r="A50" s="11" t="n">
+      <c r="A50" s="42" t="n">
         <v>36</v>
       </c>
-      <c r="B50" s="12">
+      <c r="B50" s="43">
         <f>LEFT('36'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C50" s="13">
+      <c r="C50" s="44">
         <f>'36'!H29</f>
         <v/>
       </c>
@@ -1637,14 +1672,14 @@
       <c r="I50" s="5" t="n"/>
     </row>
     <row r="51" ht="30" customHeight="1">
-      <c r="A51" s="11" t="n">
+      <c r="A51" s="42" t="n">
         <v>37</v>
       </c>
-      <c r="B51" s="12">
+      <c r="B51" s="43">
         <f>LEFT('37'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C51" s="13">
+      <c r="C51" s="44">
         <f>'37'!H29</f>
         <v/>
       </c>
@@ -1656,14 +1691,14 @@
       <c r="I51" s="5" t="n"/>
     </row>
     <row r="52" ht="30" customHeight="1">
-      <c r="A52" s="11" t="n">
+      <c r="A52" s="42" t="n">
         <v>38</v>
       </c>
-      <c r="B52" s="12">
+      <c r="B52" s="43">
         <f>LEFT('38'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C52" s="13">
+      <c r="C52" s="44">
         <f>'38'!H29</f>
         <v/>
       </c>
@@ -1675,14 +1710,14 @@
       <c r="I52" s="5" t="n"/>
     </row>
     <row r="53" ht="30" customHeight="1">
-      <c r="A53" s="11" t="n">
+      <c r="A53" s="42" t="n">
         <v>39</v>
       </c>
-      <c r="B53" s="12">
+      <c r="B53" s="43">
         <f>LEFT('39'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C53" s="13">
+      <c r="C53" s="44">
         <f>'39'!H29</f>
         <v/>
       </c>
@@ -1694,14 +1729,14 @@
       <c r="I53" s="5" t="n"/>
     </row>
     <row r="54" ht="30" customHeight="1">
-      <c r="A54" s="11" t="n">
+      <c r="A54" s="42" t="n">
         <v>40</v>
       </c>
-      <c r="B54" s="12">
+      <c r="B54" s="43">
         <f>LEFT('40'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C54" s="13">
+      <c r="C54" s="44">
         <f>'40'!H29</f>
         <v/>
       </c>
@@ -1713,14 +1748,14 @@
       <c r="I54" s="5" t="n"/>
     </row>
     <row r="55" ht="30" customHeight="1">
-      <c r="A55" s="11" t="n">
+      <c r="A55" s="42" t="n">
         <v>41</v>
       </c>
-      <c r="B55" s="12">
+      <c r="B55" s="43">
         <f>LEFT('41'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C55" s="13">
+      <c r="C55" s="44">
         <f>'41'!H29</f>
         <v/>
       </c>
@@ -1732,14 +1767,14 @@
       <c r="I55" s="5" t="n"/>
     </row>
     <row r="56" ht="30" customHeight="1">
-      <c r="A56" s="11" t="n">
+      <c r="A56" s="42" t="n">
         <v>42</v>
       </c>
-      <c r="B56" s="12">
+      <c r="B56" s="43">
         <f>LEFT('42'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C56" s="13">
+      <c r="C56" s="44">
         <f>'42'!H29</f>
         <v/>
       </c>
@@ -1751,14 +1786,14 @@
       <c r="I56" s="5" t="n"/>
     </row>
     <row r="57" ht="30" customHeight="1">
-      <c r="A57" s="11" t="n">
+      <c r="A57" s="42" t="n">
         <v>43</v>
       </c>
-      <c r="B57" s="12">
+      <c r="B57" s="43">
         <f>LEFT('43'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C57" s="13">
+      <c r="C57" s="44">
         <f>'43'!H29</f>
         <v/>
       </c>
@@ -1770,14 +1805,14 @@
       <c r="I57" s="5" t="n"/>
     </row>
     <row r="58" ht="30" customHeight="1">
-      <c r="A58" s="11" t="n">
+      <c r="A58" s="42" t="n">
         <v>44</v>
       </c>
-      <c r="B58" s="12">
+      <c r="B58" s="43">
         <f>LEFT('44'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C58" s="13">
+      <c r="C58" s="44">
         <f>'44'!H29</f>
         <v/>
       </c>
@@ -1789,14 +1824,14 @@
       <c r="I58" s="5" t="n"/>
     </row>
     <row r="59" ht="30" customHeight="1">
-      <c r="A59" s="11" t="n">
+      <c r="A59" s="42" t="n">
         <v>45</v>
       </c>
-      <c r="B59" s="12">
+      <c r="B59" s="43">
         <f>LEFT('45'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C59" s="13">
+      <c r="C59" s="44">
         <f>'45'!H29</f>
         <v/>
       </c>
@@ -1808,14 +1843,14 @@
       <c r="I59" s="5" t="n"/>
     </row>
     <row r="60" ht="30" customHeight="1">
-      <c r="A60" s="11" t="n">
+      <c r="A60" s="42" t="n">
         <v>46</v>
       </c>
-      <c r="B60" s="12">
+      <c r="B60" s="43">
         <f>LEFT('46'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C60" s="13">
+      <c r="C60" s="44">
         <f>'46'!H29</f>
         <v/>
       </c>
@@ -1827,63 +1862,62 @@
       <c r="I60" s="5" t="n"/>
     </row>
     <row r="61" ht="30" customHeight="1">
-      <c r="A61" s="11" t="n">
+      <c r="A61" s="42" t="n">
         <v>47</v>
       </c>
-      <c r="B61" s="12">
+      <c r="B61" s="43">
         <f>LEFT('47'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C61" s="13">
+      <c r="C61" s="44">
         <f>'47'!H29</f>
         <v/>
       </c>
     </row>
     <row r="62" ht="30" customHeight="1">
-      <c r="A62" s="11" t="n">
+      <c r="A62" s="42" t="n">
         <v>48</v>
       </c>
-      <c r="B62" s="12">
+      <c r="B62" s="43">
         <f>LEFT('48'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C62" s="13">
+      <c r="C62" s="44">
         <f>'48'!H29</f>
         <v/>
       </c>
     </row>
     <row r="63" ht="30" customHeight="1">
-      <c r="A63" s="11" t="n">
+      <c r="A63" s="42" t="n">
         <v>49</v>
       </c>
-      <c r="B63" s="12">
+      <c r="B63" s="43">
         <f>LEFT('49'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C63" s="13">
+      <c r="C63" s="44">
         <f>'49'!H29</f>
         <v/>
       </c>
     </row>
     <row r="64" ht="30" customHeight="1">
-      <c r="A64" s="11" t="n">
+      <c r="A64" s="42" t="n">
         <v>50</v>
       </c>
-      <c r="B64" s="12">
+      <c r="B64" s="43">
         <f>LEFT('50'!A4, 200)</f>
         <v/>
       </c>
-      <c r="C64" s="13">
+      <c r="C64" s="44">
         <f>'50'!H29</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B13:C13"/>
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B3:C3"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation sqref="D7:I7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select ✓ or X" promptTitle="Database Selection" prompt="Click to select ✓ or X" type="list">

</xml_diff>

<commit_message>
Fix dropdown validation and remove extra borders
Fixed three issues:
1. Removed dropdown validation from column C (should only be in B6:B11)
2. Cleaned up column C rows 6-11 (removed borders and fills)
3. Removed all stray borders from columns D-I throughout sheet

Now only B6:B11 has dropdown validation for database selection.
Clean 3-column layout (A, B, C) with no extra borders.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/user_testing_template.xlsx
+++ b/user_testing_template.xlsx
@@ -279,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -387,6 +387,7 @@
     <xf numFmtId="164" fontId="7" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -779,23 +780,23 @@
       </c>
       <c r="B1" s="17" t="n"/>
       <c r="C1" s="18" t="n"/>
-      <c r="D1" s="30" t="n"/>
-      <c r="E1" s="30" t="n"/>
-      <c r="F1" s="30" t="n"/>
-      <c r="G1" s="30" t="n"/>
-      <c r="H1" s="30" t="n"/>
-      <c r="I1" s="30" t="n"/>
+      <c r="D1" s="38" t="n"/>
+      <c r="E1" s="38" t="n"/>
+      <c r="F1" s="38" t="n"/>
+      <c r="G1" s="38" t="n"/>
+      <c r="H1" s="38" t="n"/>
+      <c r="I1" s="38" t="n"/>
     </row>
     <row r="2" ht="10" customHeight="1">
       <c r="A2" s="30" t="n"/>
       <c r="B2" s="30" t="n"/>
       <c r="C2" s="30" t="n"/>
-      <c r="D2" s="30" t="n"/>
-      <c r="E2" s="30" t="n"/>
-      <c r="F2" s="30" t="n"/>
-      <c r="G2" s="30" t="n"/>
-      <c r="H2" s="30" t="n"/>
-      <c r="I2" s="30" t="n"/>
+      <c r="D2" s="38" t="n"/>
+      <c r="E2" s="38" t="n"/>
+      <c r="F2" s="38" t="n"/>
+      <c r="G2" s="38" t="n"/>
+      <c r="H2" s="38" t="n"/>
+      <c r="I2" s="38" t="n"/>
     </row>
     <row r="3" ht="30" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
@@ -809,23 +810,23 @@
         </is>
       </c>
       <c r="C3" s="18" t="n"/>
-      <c r="D3" s="30" t="n"/>
-      <c r="E3" s="30" t="n"/>
-      <c r="F3" s="30" t="n"/>
-      <c r="G3" s="30" t="n"/>
-      <c r="H3" s="30" t="n"/>
-      <c r="I3" s="30" t="n"/>
+      <c r="D3" s="38" t="n"/>
+      <c r="E3" s="38" t="n"/>
+      <c r="F3" s="38" t="n"/>
+      <c r="G3" s="38" t="n"/>
+      <c r="H3" s="38" t="n"/>
+      <c r="I3" s="38" t="n"/>
     </row>
     <row r="4" ht="10" customHeight="1">
       <c r="A4" s="30" t="n"/>
       <c r="B4" s="30" t="n"/>
       <c r="C4" s="30" t="n"/>
-      <c r="D4" s="30" t="n"/>
-      <c r="E4" s="30" t="n"/>
-      <c r="F4" s="30" t="n"/>
-      <c r="G4" s="30" t="n"/>
-      <c r="H4" s="30" t="n"/>
-      <c r="I4" s="30" t="n"/>
+      <c r="D4" s="38" t="n"/>
+      <c r="E4" s="38" t="n"/>
+      <c r="F4" s="38" t="n"/>
+      <c r="G4" s="38" t="n"/>
+      <c r="H4" s="38" t="n"/>
+      <c r="I4" s="38" t="n"/>
     </row>
     <row r="5" ht="25" customHeight="1">
       <c r="A5" s="4" t="inlineStr">
@@ -835,12 +836,12 @@
       </c>
       <c r="B5" s="17" t="n"/>
       <c r="C5" s="18" t="n"/>
-      <c r="D5" s="30" t="n"/>
-      <c r="E5" s="30" t="n"/>
-      <c r="F5" s="30" t="n"/>
-      <c r="G5" s="30" t="n"/>
-      <c r="H5" s="30" t="n"/>
-      <c r="I5" s="30" t="n"/>
+      <c r="D5" s="38" t="n"/>
+      <c r="E5" s="38" t="n"/>
+      <c r="F5" s="38" t="n"/>
+      <c r="G5" s="38" t="n"/>
+      <c r="H5" s="38" t="n"/>
+      <c r="I5" s="38" t="n"/>
     </row>
     <row r="6" ht="25" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
@@ -850,12 +851,12 @@
       </c>
       <c r="B6" s="31" t="inlineStr"/>
       <c r="C6" s="37" t="n"/>
-      <c r="D6" s="28" t="n"/>
-      <c r="E6" s="28" t="n"/>
-      <c r="F6" s="28" t="n"/>
-      <c r="G6" s="28" t="n"/>
-      <c r="H6" s="28" t="n"/>
-      <c r="I6" s="28" t="n"/>
+      <c r="D6" s="37" t="n"/>
+      <c r="E6" s="37" t="n"/>
+      <c r="F6" s="37" t="n"/>
+      <c r="G6" s="37" t="n"/>
+      <c r="H6" s="37" t="n"/>
+      <c r="I6" s="37" t="n"/>
     </row>
     <row r="7" ht="25" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
@@ -865,12 +866,12 @@
       </c>
       <c r="B7" s="31" t="inlineStr"/>
       <c r="C7" s="37" t="n"/>
-      <c r="D7" s="28" t="n"/>
-      <c r="E7" s="28" t="n"/>
-      <c r="F7" s="28" t="n"/>
-      <c r="G7" s="28" t="n"/>
-      <c r="H7" s="28" t="n"/>
-      <c r="I7" s="28" t="n"/>
+      <c r="D7" s="37" t="n"/>
+      <c r="E7" s="37" t="n"/>
+      <c r="F7" s="37" t="n"/>
+      <c r="G7" s="37" t="n"/>
+      <c r="H7" s="37" t="n"/>
+      <c r="I7" s="37" t="n"/>
     </row>
     <row r="8" ht="25" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
@@ -880,12 +881,12 @@
       </c>
       <c r="B8" s="31" t="inlineStr"/>
       <c r="C8" s="38" t="n"/>
-      <c r="D8" s="30" t="n"/>
-      <c r="E8" s="30" t="n"/>
-      <c r="F8" s="30" t="n"/>
-      <c r="G8" s="30" t="n"/>
-      <c r="H8" s="30" t="n"/>
-      <c r="I8" s="30" t="n"/>
+      <c r="D8" s="38" t="n"/>
+      <c r="E8" s="38" t="n"/>
+      <c r="F8" s="38" t="n"/>
+      <c r="G8" s="38" t="n"/>
+      <c r="H8" s="38" t="n"/>
+      <c r="I8" s="38" t="n"/>
     </row>
     <row r="9" ht="25" customHeight="1">
       <c r="A9" s="2" t="inlineStr">
@@ -895,12 +896,12 @@
       </c>
       <c r="B9" s="32" t="inlineStr"/>
       <c r="C9" s="38" t="n"/>
-      <c r="D9" s="30" t="n"/>
-      <c r="E9" s="30" t="n"/>
-      <c r="F9" s="30" t="n"/>
-      <c r="G9" s="30" t="n"/>
-      <c r="H9" s="30" t="n"/>
-      <c r="I9" s="30" t="n"/>
+      <c r="D9" s="38" t="n"/>
+      <c r="E9" s="38" t="n"/>
+      <c r="F9" s="38" t="n"/>
+      <c r="G9" s="38" t="n"/>
+      <c r="H9" s="38" t="n"/>
+      <c r="I9" s="38" t="n"/>
     </row>
     <row r="10" ht="25" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
@@ -910,12 +911,12 @@
       </c>
       <c r="B10" s="31" t="inlineStr"/>
       <c r="C10" s="37" t="n"/>
-      <c r="D10" s="30" t="n"/>
-      <c r="E10" s="30" t="n"/>
-      <c r="F10" s="30" t="n"/>
-      <c r="G10" s="30" t="n"/>
-      <c r="H10" s="30" t="n"/>
-      <c r="I10" s="30" t="n"/>
+      <c r="D10" s="38" t="n"/>
+      <c r="E10" s="38" t="n"/>
+      <c r="F10" s="38" t="n"/>
+      <c r="G10" s="38" t="n"/>
+      <c r="H10" s="38" t="n"/>
+      <c r="I10" s="38" t="n"/>
     </row>
     <row r="11" ht="25" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
@@ -925,23 +926,23 @@
       </c>
       <c r="B11" s="31" t="inlineStr"/>
       <c r="C11" s="39" t="n"/>
-      <c r="D11" s="30" t="n"/>
-      <c r="E11" s="30" t="n"/>
-      <c r="F11" s="30" t="n"/>
-      <c r="G11" s="30" t="n"/>
-      <c r="H11" s="30" t="n"/>
-      <c r="I11" s="30" t="n"/>
+      <c r="D11" s="38" t="n"/>
+      <c r="E11" s="38" t="n"/>
+      <c r="F11" s="38" t="n"/>
+      <c r="G11" s="38" t="n"/>
+      <c r="H11" s="38" t="n"/>
+      <c r="I11" s="38" t="n"/>
     </row>
     <row r="12" ht="10" customHeight="1">
       <c r="A12" s="28" t="n"/>
       <c r="B12" s="34" t="n"/>
       <c r="C12" s="33" t="n"/>
-      <c r="D12" s="30" t="n"/>
-      <c r="E12" s="30" t="n"/>
-      <c r="F12" s="30" t="n"/>
-      <c r="G12" s="30" t="n"/>
-      <c r="H12" s="30" t="n"/>
-      <c r="I12" s="30" t="n"/>
+      <c r="D12" s="38" t="n"/>
+      <c r="E12" s="38" t="n"/>
+      <c r="F12" s="38" t="n"/>
+      <c r="G12" s="38" t="n"/>
+      <c r="H12" s="38" t="n"/>
+      <c r="I12" s="38" t="n"/>
     </row>
     <row r="13" ht="25" customHeight="1">
       <c r="A13" s="8" t="inlineStr">
@@ -957,12 +958,12 @@
         <f>IFERROR(AVERAGEIF(C15:C64,"&gt;0")/10,"-")</f>
         <v/>
       </c>
-      <c r="D13" s="30" t="n"/>
-      <c r="E13" s="30" t="n"/>
-      <c r="F13" s="30" t="n"/>
-      <c r="G13" s="30" t="n"/>
-      <c r="H13" s="30" t="n"/>
-      <c r="I13" s="30" t="n"/>
+      <c r="D13" s="38" t="n"/>
+      <c r="E13" s="38" t="n"/>
+      <c r="F13" s="38" t="n"/>
+      <c r="G13" s="38" t="n"/>
+      <c r="H13" s="38" t="n"/>
+      <c r="I13" s="38" t="n"/>
     </row>
     <row r="14" ht="25" customHeight="1">
       <c r="A14" s="10" t="inlineStr">
@@ -980,12 +981,12 @@
           <t>Score</t>
         </is>
       </c>
-      <c r="D14" s="30" t="n"/>
-      <c r="E14" s="30" t="n"/>
-      <c r="F14" s="30" t="n"/>
-      <c r="G14" s="30" t="n"/>
-      <c r="H14" s="30" t="n"/>
-      <c r="I14" s="30" t="n"/>
+      <c r="D14" s="38" t="n"/>
+      <c r="E14" s="38" t="n"/>
+      <c r="F14" s="38" t="n"/>
+      <c r="G14" s="38" t="n"/>
+      <c r="H14" s="38" t="n"/>
+      <c r="I14" s="38" t="n"/>
     </row>
     <row r="15" ht="30" customHeight="1">
       <c r="A15" s="42" t="n">
@@ -999,12 +1000,12 @@
         <f>'1'!H29</f>
         <v/>
       </c>
-      <c r="D15" s="30" t="n"/>
-      <c r="E15" s="30" t="n"/>
-      <c r="F15" s="30" t="n"/>
-      <c r="G15" s="30" t="n"/>
-      <c r="H15" s="30" t="n"/>
-      <c r="I15" s="30" t="n"/>
+      <c r="D15" s="38" t="n"/>
+      <c r="E15" s="38" t="n"/>
+      <c r="F15" s="38" t="n"/>
+      <c r="G15" s="38" t="n"/>
+      <c r="H15" s="38" t="n"/>
+      <c r="I15" s="38" t="n"/>
     </row>
     <row r="16" ht="30" customHeight="1">
       <c r="A16" s="42" t="n">
@@ -1018,12 +1019,12 @@
         <f>'2'!H29</f>
         <v/>
       </c>
-      <c r="D16" s="30" t="n"/>
-      <c r="E16" s="30" t="n"/>
-      <c r="F16" s="30" t="n"/>
-      <c r="G16" s="30" t="n"/>
-      <c r="H16" s="30" t="n"/>
-      <c r="I16" s="30" t="n"/>
+      <c r="D16" s="38" t="n"/>
+      <c r="E16" s="38" t="n"/>
+      <c r="F16" s="38" t="n"/>
+      <c r="G16" s="38" t="n"/>
+      <c r="H16" s="38" t="n"/>
+      <c r="I16" s="38" t="n"/>
     </row>
     <row r="17" ht="30" customHeight="1">
       <c r="A17" s="42" t="n">
@@ -1037,12 +1038,12 @@
         <f>'3'!H29</f>
         <v/>
       </c>
-      <c r="D17" s="30" t="n"/>
-      <c r="E17" s="30" t="n"/>
-      <c r="F17" s="30" t="n"/>
-      <c r="G17" s="30" t="n"/>
-      <c r="H17" s="30" t="n"/>
-      <c r="I17" s="30" t="n"/>
+      <c r="D17" s="38" t="n"/>
+      <c r="E17" s="38" t="n"/>
+      <c r="F17" s="38" t="n"/>
+      <c r="G17" s="38" t="n"/>
+      <c r="H17" s="38" t="n"/>
+      <c r="I17" s="38" t="n"/>
     </row>
     <row r="18" ht="30" customHeight="1">
       <c r="A18" s="42" t="n">
@@ -1056,12 +1057,12 @@
         <f>'4'!H29</f>
         <v/>
       </c>
-      <c r="D18" s="30" t="n"/>
-      <c r="E18" s="30" t="n"/>
-      <c r="F18" s="30" t="n"/>
-      <c r="G18" s="30" t="n"/>
-      <c r="H18" s="30" t="n"/>
-      <c r="I18" s="30" t="n"/>
+      <c r="D18" s="38" t="n"/>
+      <c r="E18" s="38" t="n"/>
+      <c r="F18" s="38" t="n"/>
+      <c r="G18" s="38" t="n"/>
+      <c r="H18" s="38" t="n"/>
+      <c r="I18" s="38" t="n"/>
     </row>
     <row r="19" ht="30" customHeight="1">
       <c r="A19" s="42" t="n">
@@ -1075,12 +1076,12 @@
         <f>'5'!H29</f>
         <v/>
       </c>
-      <c r="D19" s="30" t="n"/>
-      <c r="E19" s="30" t="n"/>
-      <c r="F19" s="30" t="n"/>
-      <c r="G19" s="30" t="n"/>
-      <c r="H19" s="30" t="n"/>
-      <c r="I19" s="30" t="n"/>
+      <c r="D19" s="38" t="n"/>
+      <c r="E19" s="38" t="n"/>
+      <c r="F19" s="38" t="n"/>
+      <c r="G19" s="38" t="n"/>
+      <c r="H19" s="38" t="n"/>
+      <c r="I19" s="38" t="n"/>
     </row>
     <row r="20" ht="30" customHeight="1">
       <c r="A20" s="42" t="n">
@@ -1094,12 +1095,12 @@
         <f>'6'!H29</f>
         <v/>
       </c>
-      <c r="D20" s="30" t="n"/>
-      <c r="E20" s="30" t="n"/>
-      <c r="F20" s="30" t="n"/>
-      <c r="G20" s="30" t="n"/>
-      <c r="H20" s="30" t="n"/>
-      <c r="I20" s="30" t="n"/>
+      <c r="D20" s="38" t="n"/>
+      <c r="E20" s="38" t="n"/>
+      <c r="F20" s="38" t="n"/>
+      <c r="G20" s="38" t="n"/>
+      <c r="H20" s="38" t="n"/>
+      <c r="I20" s="38" t="n"/>
     </row>
     <row r="21" ht="30" customHeight="1">
       <c r="A21" s="42" t="n">
@@ -1113,12 +1114,12 @@
         <f>'7'!H29</f>
         <v/>
       </c>
-      <c r="D21" s="5" t="n"/>
-      <c r="E21" s="5" t="n"/>
-      <c r="F21" s="5" t="n"/>
-      <c r="G21" s="5" t="n"/>
-      <c r="H21" s="5" t="n"/>
-      <c r="I21" s="5" t="n"/>
+      <c r="D21" s="45" t="n"/>
+      <c r="E21" s="45" t="n"/>
+      <c r="F21" s="45" t="n"/>
+      <c r="G21" s="45" t="n"/>
+      <c r="H21" s="45" t="n"/>
+      <c r="I21" s="45" t="n"/>
     </row>
     <row r="22" ht="30" customHeight="1">
       <c r="A22" s="42" t="n">
@@ -1132,12 +1133,12 @@
         <f>'8'!H29</f>
         <v/>
       </c>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
-      <c r="I22" s="5" t="n"/>
+      <c r="D22" s="45" t="n"/>
+      <c r="E22" s="45" t="n"/>
+      <c r="F22" s="45" t="n"/>
+      <c r="G22" s="45" t="n"/>
+      <c r="H22" s="45" t="n"/>
+      <c r="I22" s="45" t="n"/>
     </row>
     <row r="23" ht="30" customHeight="1">
       <c r="A23" s="42" t="n">
@@ -1151,12 +1152,12 @@
         <f>'9'!H29</f>
         <v/>
       </c>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
-      <c r="I23" s="5" t="n"/>
+      <c r="D23" s="45" t="n"/>
+      <c r="E23" s="45" t="n"/>
+      <c r="F23" s="45" t="n"/>
+      <c r="G23" s="45" t="n"/>
+      <c r="H23" s="45" t="n"/>
+      <c r="I23" s="45" t="n"/>
     </row>
     <row r="24" ht="30" customHeight="1">
       <c r="A24" s="42" t="n">
@@ -1170,12 +1171,12 @@
         <f>'10'!H29</f>
         <v/>
       </c>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
-      <c r="I24" s="5" t="n"/>
+      <c r="D24" s="45" t="n"/>
+      <c r="E24" s="45" t="n"/>
+      <c r="F24" s="45" t="n"/>
+      <c r="G24" s="45" t="n"/>
+      <c r="H24" s="45" t="n"/>
+      <c r="I24" s="45" t="n"/>
     </row>
     <row r="25" ht="30" customHeight="1">
       <c r="A25" s="42" t="n">
@@ -1189,12 +1190,12 @@
         <f>'11'!H29</f>
         <v/>
       </c>
-      <c r="D25" s="5" t="n"/>
-      <c r="E25" s="5" t="n"/>
-      <c r="F25" s="5" t="n"/>
-      <c r="G25" s="5" t="n"/>
-      <c r="H25" s="5" t="n"/>
-      <c r="I25" s="5" t="n"/>
+      <c r="D25" s="45" t="n"/>
+      <c r="E25" s="45" t="n"/>
+      <c r="F25" s="45" t="n"/>
+      <c r="G25" s="45" t="n"/>
+      <c r="H25" s="45" t="n"/>
+      <c r="I25" s="45" t="n"/>
     </row>
     <row r="26" ht="30" customHeight="1">
       <c r="A26" s="42" t="n">
@@ -1208,12 +1209,12 @@
         <f>'12'!H29</f>
         <v/>
       </c>
-      <c r="D26" s="5" t="n"/>
-      <c r="E26" s="5" t="n"/>
-      <c r="F26" s="5" t="n"/>
-      <c r="G26" s="5" t="n"/>
-      <c r="H26" s="5" t="n"/>
-      <c r="I26" s="5" t="n"/>
+      <c r="D26" s="45" t="n"/>
+      <c r="E26" s="45" t="n"/>
+      <c r="F26" s="45" t="n"/>
+      <c r="G26" s="45" t="n"/>
+      <c r="H26" s="45" t="n"/>
+      <c r="I26" s="45" t="n"/>
     </row>
     <row r="27" ht="30" customHeight="1">
       <c r="A27" s="42" t="n">
@@ -1227,12 +1228,12 @@
         <f>'13'!H29</f>
         <v/>
       </c>
-      <c r="D27" s="5" t="n"/>
-      <c r="E27" s="5" t="n"/>
-      <c r="F27" s="5" t="n"/>
-      <c r="G27" s="5" t="n"/>
-      <c r="H27" s="5" t="n"/>
-      <c r="I27" s="5" t="n"/>
+      <c r="D27" s="45" t="n"/>
+      <c r="E27" s="45" t="n"/>
+      <c r="F27" s="45" t="n"/>
+      <c r="G27" s="45" t="n"/>
+      <c r="H27" s="45" t="n"/>
+      <c r="I27" s="45" t="n"/>
     </row>
     <row r="28" ht="30" customHeight="1">
       <c r="A28" s="42" t="n">
@@ -1246,12 +1247,12 @@
         <f>'14'!H29</f>
         <v/>
       </c>
-      <c r="D28" s="5" t="n"/>
-      <c r="E28" s="5" t="n"/>
-      <c r="F28" s="5" t="n"/>
-      <c r="G28" s="5" t="n"/>
-      <c r="H28" s="5" t="n"/>
-      <c r="I28" s="5" t="n"/>
+      <c r="D28" s="45" t="n"/>
+      <c r="E28" s="45" t="n"/>
+      <c r="F28" s="45" t="n"/>
+      <c r="G28" s="45" t="n"/>
+      <c r="H28" s="45" t="n"/>
+      <c r="I28" s="45" t="n"/>
     </row>
     <row r="29" ht="30" customHeight="1">
       <c r="A29" s="42" t="n">
@@ -1265,12 +1266,12 @@
         <f>'15'!H29</f>
         <v/>
       </c>
-      <c r="D29" s="5" t="n"/>
-      <c r="E29" s="5" t="n"/>
-      <c r="F29" s="5" t="n"/>
-      <c r="G29" s="5" t="n"/>
-      <c r="H29" s="5" t="n"/>
-      <c r="I29" s="5" t="n"/>
+      <c r="D29" s="45" t="n"/>
+      <c r="E29" s="45" t="n"/>
+      <c r="F29" s="45" t="n"/>
+      <c r="G29" s="45" t="n"/>
+      <c r="H29" s="45" t="n"/>
+      <c r="I29" s="45" t="n"/>
     </row>
     <row r="30" ht="30" customHeight="1">
       <c r="A30" s="42" t="n">
@@ -1284,12 +1285,12 @@
         <f>'16'!H29</f>
         <v/>
       </c>
-      <c r="D30" s="5" t="n"/>
-      <c r="E30" s="5" t="n"/>
-      <c r="F30" s="5" t="n"/>
-      <c r="G30" s="5" t="n"/>
-      <c r="H30" s="5" t="n"/>
-      <c r="I30" s="5" t="n"/>
+      <c r="D30" s="45" t="n"/>
+      <c r="E30" s="45" t="n"/>
+      <c r="F30" s="45" t="n"/>
+      <c r="G30" s="45" t="n"/>
+      <c r="H30" s="45" t="n"/>
+      <c r="I30" s="45" t="n"/>
     </row>
     <row r="31" ht="30" customHeight="1">
       <c r="A31" s="42" t="n">
@@ -1303,12 +1304,12 @@
         <f>'17'!H29</f>
         <v/>
       </c>
-      <c r="D31" s="5" t="n"/>
-      <c r="E31" s="5" t="n"/>
-      <c r="F31" s="5" t="n"/>
-      <c r="G31" s="5" t="n"/>
-      <c r="H31" s="5" t="n"/>
-      <c r="I31" s="5" t="n"/>
+      <c r="D31" s="45" t="n"/>
+      <c r="E31" s="45" t="n"/>
+      <c r="F31" s="45" t="n"/>
+      <c r="G31" s="45" t="n"/>
+      <c r="H31" s="45" t="n"/>
+      <c r="I31" s="45" t="n"/>
     </row>
     <row r="32" ht="30" customHeight="1">
       <c r="A32" s="42" t="n">
@@ -1322,12 +1323,12 @@
         <f>'18'!H29</f>
         <v/>
       </c>
-      <c r="D32" s="5" t="n"/>
-      <c r="E32" s="5" t="n"/>
-      <c r="F32" s="5" t="n"/>
-      <c r="G32" s="5" t="n"/>
-      <c r="H32" s="5" t="n"/>
-      <c r="I32" s="5" t="n"/>
+      <c r="D32" s="45" t="n"/>
+      <c r="E32" s="45" t="n"/>
+      <c r="F32" s="45" t="n"/>
+      <c r="G32" s="45" t="n"/>
+      <c r="H32" s="45" t="n"/>
+      <c r="I32" s="45" t="n"/>
     </row>
     <row r="33" ht="30" customHeight="1">
       <c r="A33" s="42" t="n">
@@ -1341,12 +1342,12 @@
         <f>'19'!H29</f>
         <v/>
       </c>
-      <c r="D33" s="5" t="n"/>
-      <c r="E33" s="5" t="n"/>
-      <c r="F33" s="5" t="n"/>
-      <c r="G33" s="5" t="n"/>
-      <c r="H33" s="5" t="n"/>
-      <c r="I33" s="5" t="n"/>
+      <c r="D33" s="45" t="n"/>
+      <c r="E33" s="45" t="n"/>
+      <c r="F33" s="45" t="n"/>
+      <c r="G33" s="45" t="n"/>
+      <c r="H33" s="45" t="n"/>
+      <c r="I33" s="45" t="n"/>
     </row>
     <row r="34" ht="30" customHeight="1">
       <c r="A34" s="42" t="n">
@@ -1360,12 +1361,12 @@
         <f>'20'!H29</f>
         <v/>
       </c>
-      <c r="D34" s="5" t="n"/>
-      <c r="E34" s="5" t="n"/>
-      <c r="F34" s="5" t="n"/>
-      <c r="G34" s="5" t="n"/>
-      <c r="H34" s="5" t="n"/>
-      <c r="I34" s="5" t="n"/>
+      <c r="D34" s="45" t="n"/>
+      <c r="E34" s="45" t="n"/>
+      <c r="F34" s="45" t="n"/>
+      <c r="G34" s="45" t="n"/>
+      <c r="H34" s="45" t="n"/>
+      <c r="I34" s="45" t="n"/>
     </row>
     <row r="35" ht="30" customHeight="1">
       <c r="A35" s="42" t="n">
@@ -1379,12 +1380,12 @@
         <f>'21'!H29</f>
         <v/>
       </c>
-      <c r="D35" s="5" t="n"/>
-      <c r="E35" s="5" t="n"/>
-      <c r="F35" s="5" t="n"/>
-      <c r="G35" s="5" t="n"/>
-      <c r="H35" s="5" t="n"/>
-      <c r="I35" s="5" t="n"/>
+      <c r="D35" s="45" t="n"/>
+      <c r="E35" s="45" t="n"/>
+      <c r="F35" s="45" t="n"/>
+      <c r="G35" s="45" t="n"/>
+      <c r="H35" s="45" t="n"/>
+      <c r="I35" s="45" t="n"/>
     </row>
     <row r="36" ht="30" customHeight="1">
       <c r="A36" s="42" t="n">
@@ -1398,12 +1399,12 @@
         <f>'22'!H29</f>
         <v/>
       </c>
-      <c r="D36" s="5" t="n"/>
-      <c r="E36" s="5" t="n"/>
-      <c r="F36" s="5" t="n"/>
-      <c r="G36" s="5" t="n"/>
-      <c r="H36" s="5" t="n"/>
-      <c r="I36" s="5" t="n"/>
+      <c r="D36" s="45" t="n"/>
+      <c r="E36" s="45" t="n"/>
+      <c r="F36" s="45" t="n"/>
+      <c r="G36" s="45" t="n"/>
+      <c r="H36" s="45" t="n"/>
+      <c r="I36" s="45" t="n"/>
     </row>
     <row r="37" ht="30" customHeight="1">
       <c r="A37" s="42" t="n">
@@ -1417,12 +1418,12 @@
         <f>'23'!H29</f>
         <v/>
       </c>
-      <c r="D37" s="5" t="n"/>
-      <c r="E37" s="5" t="n"/>
-      <c r="F37" s="5" t="n"/>
-      <c r="G37" s="5" t="n"/>
-      <c r="H37" s="5" t="n"/>
-      <c r="I37" s="5" t="n"/>
+      <c r="D37" s="45" t="n"/>
+      <c r="E37" s="45" t="n"/>
+      <c r="F37" s="45" t="n"/>
+      <c r="G37" s="45" t="n"/>
+      <c r="H37" s="45" t="n"/>
+      <c r="I37" s="45" t="n"/>
     </row>
     <row r="38" ht="30" customHeight="1">
       <c r="A38" s="42" t="n">
@@ -1436,12 +1437,12 @@
         <f>'24'!H29</f>
         <v/>
       </c>
-      <c r="D38" s="5" t="n"/>
-      <c r="E38" s="5" t="n"/>
-      <c r="F38" s="5" t="n"/>
-      <c r="G38" s="5" t="n"/>
-      <c r="H38" s="5" t="n"/>
-      <c r="I38" s="5" t="n"/>
+      <c r="D38" s="45" t="n"/>
+      <c r="E38" s="45" t="n"/>
+      <c r="F38" s="45" t="n"/>
+      <c r="G38" s="45" t="n"/>
+      <c r="H38" s="45" t="n"/>
+      <c r="I38" s="45" t="n"/>
     </row>
     <row r="39" ht="30" customHeight="1">
       <c r="A39" s="42" t="n">
@@ -1455,12 +1456,12 @@
         <f>'25'!H29</f>
         <v/>
       </c>
-      <c r="D39" s="5" t="n"/>
-      <c r="E39" s="5" t="n"/>
-      <c r="F39" s="5" t="n"/>
-      <c r="G39" s="5" t="n"/>
-      <c r="H39" s="5" t="n"/>
-      <c r="I39" s="5" t="n"/>
+      <c r="D39" s="45" t="n"/>
+      <c r="E39" s="45" t="n"/>
+      <c r="F39" s="45" t="n"/>
+      <c r="G39" s="45" t="n"/>
+      <c r="H39" s="45" t="n"/>
+      <c r="I39" s="45" t="n"/>
     </row>
     <row r="40" ht="30" customHeight="1">
       <c r="A40" s="42" t="n">
@@ -1474,12 +1475,12 @@
         <f>'26'!H29</f>
         <v/>
       </c>
-      <c r="D40" s="5" t="n"/>
-      <c r="E40" s="5" t="n"/>
-      <c r="F40" s="5" t="n"/>
-      <c r="G40" s="5" t="n"/>
-      <c r="H40" s="5" t="n"/>
-      <c r="I40" s="5" t="n"/>
+      <c r="D40" s="45" t="n"/>
+      <c r="E40" s="45" t="n"/>
+      <c r="F40" s="45" t="n"/>
+      <c r="G40" s="45" t="n"/>
+      <c r="H40" s="45" t="n"/>
+      <c r="I40" s="45" t="n"/>
     </row>
     <row r="41" ht="30" customHeight="1">
       <c r="A41" s="42" t="n">
@@ -1493,12 +1494,12 @@
         <f>'27'!H29</f>
         <v/>
       </c>
-      <c r="D41" s="5" t="n"/>
-      <c r="E41" s="5" t="n"/>
-      <c r="F41" s="5" t="n"/>
-      <c r="G41" s="5" t="n"/>
-      <c r="H41" s="5" t="n"/>
-      <c r="I41" s="5" t="n"/>
+      <c r="D41" s="45" t="n"/>
+      <c r="E41" s="45" t="n"/>
+      <c r="F41" s="45" t="n"/>
+      <c r="G41" s="45" t="n"/>
+      <c r="H41" s="45" t="n"/>
+      <c r="I41" s="45" t="n"/>
     </row>
     <row r="42" ht="30" customHeight="1">
       <c r="A42" s="42" t="n">
@@ -1512,12 +1513,12 @@
         <f>'28'!H29</f>
         <v/>
       </c>
-      <c r="D42" s="5" t="n"/>
-      <c r="E42" s="5" t="n"/>
-      <c r="F42" s="5" t="n"/>
-      <c r="G42" s="5" t="n"/>
-      <c r="H42" s="5" t="n"/>
-      <c r="I42" s="5" t="n"/>
+      <c r="D42" s="45" t="n"/>
+      <c r="E42" s="45" t="n"/>
+      <c r="F42" s="45" t="n"/>
+      <c r="G42" s="45" t="n"/>
+      <c r="H42" s="45" t="n"/>
+      <c r="I42" s="45" t="n"/>
     </row>
     <row r="43" ht="30" customHeight="1">
       <c r="A43" s="42" t="n">
@@ -1531,12 +1532,12 @@
         <f>'29'!H29</f>
         <v/>
       </c>
-      <c r="D43" s="5" t="n"/>
-      <c r="E43" s="5" t="n"/>
-      <c r="F43" s="5" t="n"/>
-      <c r="G43" s="5" t="n"/>
-      <c r="H43" s="5" t="n"/>
-      <c r="I43" s="5" t="n"/>
+      <c r="D43" s="45" t="n"/>
+      <c r="E43" s="45" t="n"/>
+      <c r="F43" s="45" t="n"/>
+      <c r="G43" s="45" t="n"/>
+      <c r="H43" s="45" t="n"/>
+      <c r="I43" s="45" t="n"/>
     </row>
     <row r="44" ht="30" customHeight="1">
       <c r="A44" s="42" t="n">
@@ -1550,12 +1551,12 @@
         <f>'30'!H29</f>
         <v/>
       </c>
-      <c r="D44" s="5" t="n"/>
-      <c r="E44" s="5" t="n"/>
-      <c r="F44" s="5" t="n"/>
-      <c r="G44" s="5" t="n"/>
-      <c r="H44" s="5" t="n"/>
-      <c r="I44" s="5" t="n"/>
+      <c r="D44" s="45" t="n"/>
+      <c r="E44" s="45" t="n"/>
+      <c r="F44" s="45" t="n"/>
+      <c r="G44" s="45" t="n"/>
+      <c r="H44" s="45" t="n"/>
+      <c r="I44" s="45" t="n"/>
     </row>
     <row r="45" ht="30" customHeight="1">
       <c r="A45" s="42" t="n">
@@ -1569,12 +1570,12 @@
         <f>'31'!H29</f>
         <v/>
       </c>
-      <c r="D45" s="5" t="n"/>
-      <c r="E45" s="5" t="n"/>
-      <c r="F45" s="5" t="n"/>
-      <c r="G45" s="5" t="n"/>
-      <c r="H45" s="5" t="n"/>
-      <c r="I45" s="5" t="n"/>
+      <c r="D45" s="45" t="n"/>
+      <c r="E45" s="45" t="n"/>
+      <c r="F45" s="45" t="n"/>
+      <c r="G45" s="45" t="n"/>
+      <c r="H45" s="45" t="n"/>
+      <c r="I45" s="45" t="n"/>
     </row>
     <row r="46" ht="30" customHeight="1">
       <c r="A46" s="42" t="n">
@@ -1588,12 +1589,12 @@
         <f>'32'!H29</f>
         <v/>
       </c>
-      <c r="D46" s="5" t="n"/>
-      <c r="E46" s="5" t="n"/>
-      <c r="F46" s="5" t="n"/>
-      <c r="G46" s="5" t="n"/>
-      <c r="H46" s="5" t="n"/>
-      <c r="I46" s="5" t="n"/>
+      <c r="D46" s="45" t="n"/>
+      <c r="E46" s="45" t="n"/>
+      <c r="F46" s="45" t="n"/>
+      <c r="G46" s="45" t="n"/>
+      <c r="H46" s="45" t="n"/>
+      <c r="I46" s="45" t="n"/>
     </row>
     <row r="47" ht="30" customHeight="1">
       <c r="A47" s="42" t="n">
@@ -1607,12 +1608,12 @@
         <f>'33'!H29</f>
         <v/>
       </c>
-      <c r="D47" s="5" t="n"/>
-      <c r="E47" s="5" t="n"/>
-      <c r="F47" s="5" t="n"/>
-      <c r="G47" s="5" t="n"/>
-      <c r="H47" s="5" t="n"/>
-      <c r="I47" s="5" t="n"/>
+      <c r="D47" s="45" t="n"/>
+      <c r="E47" s="45" t="n"/>
+      <c r="F47" s="45" t="n"/>
+      <c r="G47" s="45" t="n"/>
+      <c r="H47" s="45" t="n"/>
+      <c r="I47" s="45" t="n"/>
     </row>
     <row r="48" ht="30" customHeight="1">
       <c r="A48" s="42" t="n">
@@ -1626,12 +1627,12 @@
         <f>'34'!H29</f>
         <v/>
       </c>
-      <c r="D48" s="5" t="n"/>
-      <c r="E48" s="5" t="n"/>
-      <c r="F48" s="5" t="n"/>
-      <c r="G48" s="5" t="n"/>
-      <c r="H48" s="5" t="n"/>
-      <c r="I48" s="5" t="n"/>
+      <c r="D48" s="45" t="n"/>
+      <c r="E48" s="45" t="n"/>
+      <c r="F48" s="45" t="n"/>
+      <c r="G48" s="45" t="n"/>
+      <c r="H48" s="45" t="n"/>
+      <c r="I48" s="45" t="n"/>
     </row>
     <row r="49" ht="30" customHeight="1">
       <c r="A49" s="42" t="n">
@@ -1645,12 +1646,12 @@
         <f>'35'!H29</f>
         <v/>
       </c>
-      <c r="D49" s="5" t="n"/>
-      <c r="E49" s="5" t="n"/>
-      <c r="F49" s="5" t="n"/>
-      <c r="G49" s="5" t="n"/>
-      <c r="H49" s="5" t="n"/>
-      <c r="I49" s="5" t="n"/>
+      <c r="D49" s="45" t="n"/>
+      <c r="E49" s="45" t="n"/>
+      <c r="F49" s="45" t="n"/>
+      <c r="G49" s="45" t="n"/>
+      <c r="H49" s="45" t="n"/>
+      <c r="I49" s="45" t="n"/>
     </row>
     <row r="50" ht="30" customHeight="1">
       <c r="A50" s="42" t="n">
@@ -1664,12 +1665,12 @@
         <f>'36'!H29</f>
         <v/>
       </c>
-      <c r="D50" s="5" t="n"/>
-      <c r="E50" s="5" t="n"/>
-      <c r="F50" s="5" t="n"/>
-      <c r="G50" s="5" t="n"/>
-      <c r="H50" s="5" t="n"/>
-      <c r="I50" s="5" t="n"/>
+      <c r="D50" s="45" t="n"/>
+      <c r="E50" s="45" t="n"/>
+      <c r="F50" s="45" t="n"/>
+      <c r="G50" s="45" t="n"/>
+      <c r="H50" s="45" t="n"/>
+      <c r="I50" s="45" t="n"/>
     </row>
     <row r="51" ht="30" customHeight="1">
       <c r="A51" s="42" t="n">
@@ -1683,12 +1684,12 @@
         <f>'37'!H29</f>
         <v/>
       </c>
-      <c r="D51" s="5" t="n"/>
-      <c r="E51" s="5" t="n"/>
-      <c r="F51" s="5" t="n"/>
-      <c r="G51" s="5" t="n"/>
-      <c r="H51" s="5" t="n"/>
-      <c r="I51" s="5" t="n"/>
+      <c r="D51" s="45" t="n"/>
+      <c r="E51" s="45" t="n"/>
+      <c r="F51" s="45" t="n"/>
+      <c r="G51" s="45" t="n"/>
+      <c r="H51" s="45" t="n"/>
+      <c r="I51" s="45" t="n"/>
     </row>
     <row r="52" ht="30" customHeight="1">
       <c r="A52" s="42" t="n">
@@ -1702,12 +1703,12 @@
         <f>'38'!H29</f>
         <v/>
       </c>
-      <c r="D52" s="5" t="n"/>
-      <c r="E52" s="5" t="n"/>
-      <c r="F52" s="5" t="n"/>
-      <c r="G52" s="5" t="n"/>
-      <c r="H52" s="5" t="n"/>
-      <c r="I52" s="5" t="n"/>
+      <c r="D52" s="45" t="n"/>
+      <c r="E52" s="45" t="n"/>
+      <c r="F52" s="45" t="n"/>
+      <c r="G52" s="45" t="n"/>
+      <c r="H52" s="45" t="n"/>
+      <c r="I52" s="45" t="n"/>
     </row>
     <row r="53" ht="30" customHeight="1">
       <c r="A53" s="42" t="n">
@@ -1721,12 +1722,12 @@
         <f>'39'!H29</f>
         <v/>
       </c>
-      <c r="D53" s="5" t="n"/>
-      <c r="E53" s="5" t="n"/>
-      <c r="F53" s="5" t="n"/>
-      <c r="G53" s="5" t="n"/>
-      <c r="H53" s="5" t="n"/>
-      <c r="I53" s="5" t="n"/>
+      <c r="D53" s="45" t="n"/>
+      <c r="E53" s="45" t="n"/>
+      <c r="F53" s="45" t="n"/>
+      <c r="G53" s="45" t="n"/>
+      <c r="H53" s="45" t="n"/>
+      <c r="I53" s="45" t="n"/>
     </row>
     <row r="54" ht="30" customHeight="1">
       <c r="A54" s="42" t="n">
@@ -1740,12 +1741,12 @@
         <f>'40'!H29</f>
         <v/>
       </c>
-      <c r="D54" s="5" t="n"/>
-      <c r="E54" s="5" t="n"/>
-      <c r="F54" s="5" t="n"/>
-      <c r="G54" s="5" t="n"/>
-      <c r="H54" s="5" t="n"/>
-      <c r="I54" s="5" t="n"/>
+      <c r="D54" s="45" t="n"/>
+      <c r="E54" s="45" t="n"/>
+      <c r="F54" s="45" t="n"/>
+      <c r="G54" s="45" t="n"/>
+      <c r="H54" s="45" t="n"/>
+      <c r="I54" s="45" t="n"/>
     </row>
     <row r="55" ht="30" customHeight="1">
       <c r="A55" s="42" t="n">
@@ -1759,12 +1760,12 @@
         <f>'41'!H29</f>
         <v/>
       </c>
-      <c r="D55" s="5" t="n"/>
-      <c r="E55" s="5" t="n"/>
-      <c r="F55" s="5" t="n"/>
-      <c r="G55" s="5" t="n"/>
-      <c r="H55" s="5" t="n"/>
-      <c r="I55" s="5" t="n"/>
+      <c r="D55" s="45" t="n"/>
+      <c r="E55" s="45" t="n"/>
+      <c r="F55" s="45" t="n"/>
+      <c r="G55" s="45" t="n"/>
+      <c r="H55" s="45" t="n"/>
+      <c r="I55" s="45" t="n"/>
     </row>
     <row r="56" ht="30" customHeight="1">
       <c r="A56" s="42" t="n">
@@ -1778,12 +1779,12 @@
         <f>'42'!H29</f>
         <v/>
       </c>
-      <c r="D56" s="5" t="n"/>
-      <c r="E56" s="5" t="n"/>
-      <c r="F56" s="5" t="n"/>
-      <c r="G56" s="5" t="n"/>
-      <c r="H56" s="5" t="n"/>
-      <c r="I56" s="5" t="n"/>
+      <c r="D56" s="45" t="n"/>
+      <c r="E56" s="45" t="n"/>
+      <c r="F56" s="45" t="n"/>
+      <c r="G56" s="45" t="n"/>
+      <c r="H56" s="45" t="n"/>
+      <c r="I56" s="45" t="n"/>
     </row>
     <row r="57" ht="30" customHeight="1">
       <c r="A57" s="42" t="n">
@@ -1797,12 +1798,12 @@
         <f>'43'!H29</f>
         <v/>
       </c>
-      <c r="D57" s="5" t="n"/>
-      <c r="E57" s="5" t="n"/>
-      <c r="F57" s="5" t="n"/>
-      <c r="G57" s="5" t="n"/>
-      <c r="H57" s="5" t="n"/>
-      <c r="I57" s="5" t="n"/>
+      <c r="D57" s="45" t="n"/>
+      <c r="E57" s="45" t="n"/>
+      <c r="F57" s="45" t="n"/>
+      <c r="G57" s="45" t="n"/>
+      <c r="H57" s="45" t="n"/>
+      <c r="I57" s="45" t="n"/>
     </row>
     <row r="58" ht="30" customHeight="1">
       <c r="A58" s="42" t="n">
@@ -1816,12 +1817,12 @@
         <f>'44'!H29</f>
         <v/>
       </c>
-      <c r="D58" s="5" t="n"/>
-      <c r="E58" s="5" t="n"/>
-      <c r="F58" s="5" t="n"/>
-      <c r="G58" s="5" t="n"/>
-      <c r="H58" s="5" t="n"/>
-      <c r="I58" s="5" t="n"/>
+      <c r="D58" s="45" t="n"/>
+      <c r="E58" s="45" t="n"/>
+      <c r="F58" s="45" t="n"/>
+      <c r="G58" s="45" t="n"/>
+      <c r="H58" s="45" t="n"/>
+      <c r="I58" s="45" t="n"/>
     </row>
     <row r="59" ht="30" customHeight="1">
       <c r="A59" s="42" t="n">
@@ -1835,12 +1836,12 @@
         <f>'45'!H29</f>
         <v/>
       </c>
-      <c r="D59" s="5" t="n"/>
-      <c r="E59" s="5" t="n"/>
-      <c r="F59" s="5" t="n"/>
-      <c r="G59" s="5" t="n"/>
-      <c r="H59" s="5" t="n"/>
-      <c r="I59" s="5" t="n"/>
+      <c r="D59" s="45" t="n"/>
+      <c r="E59" s="45" t="n"/>
+      <c r="F59" s="45" t="n"/>
+      <c r="G59" s="45" t="n"/>
+      <c r="H59" s="45" t="n"/>
+      <c r="I59" s="45" t="n"/>
     </row>
     <row r="60" ht="30" customHeight="1">
       <c r="A60" s="42" t="n">
@@ -1854,12 +1855,12 @@
         <f>'46'!H29</f>
         <v/>
       </c>
-      <c r="D60" s="5" t="n"/>
-      <c r="E60" s="5" t="n"/>
-      <c r="F60" s="5" t="n"/>
-      <c r="G60" s="5" t="n"/>
-      <c r="H60" s="5" t="n"/>
-      <c r="I60" s="5" t="n"/>
+      <c r="D60" s="45" t="n"/>
+      <c r="E60" s="45" t="n"/>
+      <c r="F60" s="45" t="n"/>
+      <c r="G60" s="45" t="n"/>
+      <c r="H60" s="45" t="n"/>
+      <c r="I60" s="45" t="n"/>
     </row>
     <row r="61" ht="30" customHeight="1">
       <c r="A61" s="42" t="n">
@@ -1873,6 +1874,12 @@
         <f>'47'!H29</f>
         <v/>
       </c>
+      <c r="D61" s="45" t="n"/>
+      <c r="E61" s="45" t="n"/>
+      <c r="F61" s="45" t="n"/>
+      <c r="G61" s="45" t="n"/>
+      <c r="H61" s="45" t="n"/>
+      <c r="I61" s="45" t="n"/>
     </row>
     <row r="62" ht="30" customHeight="1">
       <c r="A62" s="42" t="n">
@@ -1886,6 +1893,12 @@
         <f>'48'!H29</f>
         <v/>
       </c>
+      <c r="D62" s="45" t="n"/>
+      <c r="E62" s="45" t="n"/>
+      <c r="F62" s="45" t="n"/>
+      <c r="G62" s="45" t="n"/>
+      <c r="H62" s="45" t="n"/>
+      <c r="I62" s="45" t="n"/>
     </row>
     <row r="63" ht="30" customHeight="1">
       <c r="A63" s="42" t="n">
@@ -1899,6 +1912,12 @@
         <f>'49'!H29</f>
         <v/>
       </c>
+      <c r="D63" s="45" t="n"/>
+      <c r="E63" s="45" t="n"/>
+      <c r="F63" s="45" t="n"/>
+      <c r="G63" s="45" t="n"/>
+      <c r="H63" s="45" t="n"/>
+      <c r="I63" s="45" t="n"/>
     </row>
     <row r="64" ht="30" customHeight="1">
       <c r="A64" s="42" t="n">
@@ -1912,6 +1931,12 @@
         <f>'50'!H29</f>
         <v/>
       </c>
+      <c r="D64" s="45" t="n"/>
+      <c r="E64" s="45" t="n"/>
+      <c r="F64" s="45" t="n"/>
+      <c r="G64" s="45" t="n"/>
+      <c r="H64" s="45" t="n"/>
+      <c r="I64" s="45" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1919,13 +1944,7 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="A5:C5"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation sqref="D7:I7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select ✓ or X" promptTitle="Database Selection" prompt="Click to select ✓ or X" type="list">
-      <formula1>"✓,X"</formula1>
-    </dataValidation>
-    <dataValidation sqref="A7:F7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select ✓ or X" promptTitle="Database Selection" prompt="Click to select ✓ or X" type="list">
-      <formula1>"✓,X"</formula1>
-    </dataValidation>
+  <dataValidations count="1">
     <dataValidation sqref="B6:B11" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select ✓ or X" promptTitle="Database Selection" prompt="Click to select ✓ or X" type="list">
       <formula1>"✓,X"</formula1>
     </dataValidation>

</xml_diff>